<commit_message>
increased timeout time to 15 minutes
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -19,1933 +19,1933 @@
     <t>"09-22-01</t>
   </si>
   <si>
-    <t>0xc0000636a0</t>
+    <t>0xc0005000c0</t>
   </si>
   <si>
     <t>PW</t>
   </si>
   <si>
-    <t>0xc000063690</t>
-  </si>
-  <si>
-    <t>0xc0000636b0</t>
-  </si>
-  <si>
-    <t>0xc0000636c0</t>
-  </si>
-  <si>
-    <t>0xc0000636d0</t>
-  </si>
-  <si>
-    <t>0xc0000243c8</t>
+    <t>0xc0005000b0</t>
+  </si>
+  <si>
+    <t>0xc0005000d0</t>
+  </si>
+  <si>
+    <t>0xc0005000e0</t>
+  </si>
+  <si>
+    <t>0xc0005000f0</t>
+  </si>
+  <si>
+    <t>0xc0005060e8</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
-    <t>0xc0000243d8</t>
+    <t>0xc0005060f8</t>
   </si>
   <si>
     <t>"09-22-03</t>
   </si>
   <si>
-    <t>0xc0000636f0</t>
-  </si>
-  <si>
-    <t>0xc0000636e0</t>
-  </si>
-  <si>
-    <t>0xc000063700</t>
-  </si>
-  <si>
-    <t>0xc000063710</t>
-  </si>
-  <si>
-    <t>0xc000063720</t>
-  </si>
-  <si>
-    <t>0xc000024410</t>
-  </si>
-  <si>
-    <t>0xc000024420</t>
+    <t>0xc000500110</t>
+  </si>
+  <si>
+    <t>0xc000500100</t>
+  </si>
+  <si>
+    <t>0xc000500120</t>
+  </si>
+  <si>
+    <t>0xc000500130</t>
+  </si>
+  <si>
+    <t>0xc000500140</t>
+  </si>
+  <si>
+    <t>0xc000506130</t>
+  </si>
+  <si>
+    <t>0xc000506140</t>
   </si>
   <si>
     <t>"09-22-04</t>
   </si>
   <si>
-    <t>0xc000063740</t>
-  </si>
-  <si>
-    <t>0xc000063730</t>
-  </si>
-  <si>
-    <t>0xc000063750</t>
-  </si>
-  <si>
-    <t>0xc000063760</t>
-  </si>
-  <si>
-    <t>0xc000063770</t>
-  </si>
-  <si>
-    <t>0xc000024458</t>
-  </si>
-  <si>
-    <t>0xc000024468</t>
+    <t>0xc000500160</t>
+  </si>
+  <si>
+    <t>0xc000500150</t>
+  </si>
+  <si>
+    <t>0xc000500170</t>
+  </si>
+  <si>
+    <t>0xc000500180</t>
+  </si>
+  <si>
+    <t>0xc000500190</t>
+  </si>
+  <si>
+    <t>0xc000506178</t>
+  </si>
+  <si>
+    <t>0xc000506188</t>
   </si>
   <si>
     <t>"09-22-05</t>
   </si>
   <si>
-    <t>0xc000063790</t>
-  </si>
-  <si>
-    <t>0xc000063780</t>
-  </si>
-  <si>
-    <t>0xc0000637a0</t>
-  </si>
-  <si>
-    <t>0xc0000637b0</t>
-  </si>
-  <si>
-    <t>0xc0000637c0</t>
-  </si>
-  <si>
-    <t>0xc000024498</t>
-  </si>
-  <si>
-    <t>0xc0000244a8</t>
+    <t>0xc0005001b0</t>
+  </si>
+  <si>
+    <t>0xc0005001a0</t>
+  </si>
+  <si>
+    <t>0xc0005001c0</t>
+  </si>
+  <si>
+    <t>0xc0005001d0</t>
+  </si>
+  <si>
+    <t>0xc0005001e0</t>
+  </si>
+  <si>
+    <t>0xc0005061b8</t>
+  </si>
+  <si>
+    <t>0xc0005061c8</t>
   </si>
   <si>
     <t>"09-22-06</t>
   </si>
   <si>
-    <t>0xc0000637e0</t>
-  </si>
-  <si>
-    <t>0xc0000637d0</t>
-  </si>
-  <si>
-    <t>0xc0000637f0</t>
-  </si>
-  <si>
-    <t>0xc000063800</t>
-  </si>
-  <si>
-    <t>0xc000063810</t>
-  </si>
-  <si>
-    <t>0xc0000244e0</t>
-  </si>
-  <si>
-    <t>0xc0000244f0</t>
+    <t>0xc000500200</t>
+  </si>
+  <si>
+    <t>0xc0005001f0</t>
+  </si>
+  <si>
+    <t>0xc000500210</t>
+  </si>
+  <si>
+    <t>0xc000500220</t>
+  </si>
+  <si>
+    <t>0xc000500230</t>
+  </si>
+  <si>
+    <t>0xc000506200</t>
+  </si>
+  <si>
+    <t>0xc000506210</t>
   </si>
   <si>
     <t>"09-22-07</t>
   </si>
   <si>
-    <t>0xc000063830</t>
-  </si>
-  <si>
-    <t>0xc000063820</t>
-  </si>
-  <si>
-    <t>0xc000063840</t>
-  </si>
-  <si>
-    <t>0xc000063850</t>
-  </si>
-  <si>
-    <t>0xc000063860</t>
-  </si>
-  <si>
-    <t>0xc000024520</t>
-  </si>
-  <si>
-    <t>0xc000024538</t>
+    <t>0xc000500250</t>
+  </si>
+  <si>
+    <t>0xc000500240</t>
+  </si>
+  <si>
+    <t>0xc000500260</t>
+  </si>
+  <si>
+    <t>0xc000500270</t>
+  </si>
+  <si>
+    <t>0xc000500280</t>
+  </si>
+  <si>
+    <t>0xc000506240</t>
+  </si>
+  <si>
+    <t>0xc000506258</t>
   </si>
   <si>
     <t>"09-22-08</t>
   </si>
   <si>
-    <t>0xc000063880</t>
-  </si>
-  <si>
-    <t>0xc000063870</t>
-  </si>
-  <si>
-    <t>0xc000063890</t>
-  </si>
-  <si>
-    <t>0xc0000638a0</t>
-  </si>
-  <si>
-    <t>0xc0000638b0</t>
-  </si>
-  <si>
-    <t>0xc000024560</t>
-  </si>
-  <si>
-    <t>0xc000024578</t>
+    <t>0xc0005002a0</t>
+  </si>
+  <si>
+    <t>0xc000500290</t>
+  </si>
+  <si>
+    <t>0xc0005002b0</t>
+  </si>
+  <si>
+    <t>0xc0005002c0</t>
+  </si>
+  <si>
+    <t>0xc0005002d0</t>
+  </si>
+  <si>
+    <t>0xc000506280</t>
+  </si>
+  <si>
+    <t>0xc000506298</t>
   </si>
   <si>
     <t>"09-22-09</t>
   </si>
   <si>
-    <t>0xc0000638d0</t>
-  </si>
-  <si>
-    <t>0xc0000638c0</t>
-  </si>
-  <si>
-    <t>0xc0000638e0</t>
-  </si>
-  <si>
-    <t>0xc0000638f0</t>
-  </si>
-  <si>
-    <t>0xc000063900</t>
-  </si>
-  <si>
-    <t>0xc0000245b8</t>
-  </si>
-  <si>
-    <t>0xc0000245d0</t>
+    <t>0xc0005002f0</t>
+  </si>
+  <si>
+    <t>0xc0005002e0</t>
+  </si>
+  <si>
+    <t>0xc000500300</t>
+  </si>
+  <si>
+    <t>0xc000500310</t>
+  </si>
+  <si>
+    <t>0xc000500320</t>
+  </si>
+  <si>
+    <t>0xc0005062d8</t>
+  </si>
+  <si>
+    <t>0xc0005062f0</t>
   </si>
   <si>
     <t>"09-22-10</t>
   </si>
   <si>
-    <t>0xc000063920</t>
-  </si>
-  <si>
-    <t>0xc000063910</t>
-  </si>
-  <si>
-    <t>0xc000063930</t>
-  </si>
-  <si>
-    <t>0xc000063940</t>
-  </si>
-  <si>
-    <t>0xc000063950</t>
-  </si>
-  <si>
-    <t>0xc000024610</t>
-  </si>
-  <si>
-    <t>0xc000024628</t>
+    <t>0xc000500340</t>
+  </si>
+  <si>
+    <t>0xc000500330</t>
+  </si>
+  <si>
+    <t>0xc000500350</t>
+  </si>
+  <si>
+    <t>0xc000500360</t>
+  </si>
+  <si>
+    <t>0xc000500370</t>
+  </si>
+  <si>
+    <t>0xc000506330</t>
+  </si>
+  <si>
+    <t>0xc000506348</t>
   </si>
   <si>
     <t>"09-22-11</t>
   </si>
   <si>
-    <t>0xc000063970</t>
-  </si>
-  <si>
-    <t>0xc000063960</t>
-  </si>
-  <si>
-    <t>0xc000063980</t>
-  </si>
-  <si>
-    <t>0xc000063990</t>
-  </si>
-  <si>
-    <t>0xc0000639a0</t>
-  </si>
-  <si>
-    <t>0xc000024660</t>
-  </si>
-  <si>
-    <t>0xc000024678</t>
+    <t>0xc000500390</t>
+  </si>
+  <si>
+    <t>0xc000500380</t>
+  </si>
+  <si>
+    <t>0xc0005003a0</t>
+  </si>
+  <si>
+    <t>0xc0005003b0</t>
+  </si>
+  <si>
+    <t>0xc0005003c0</t>
+  </si>
+  <si>
+    <t>0xc000506380</t>
+  </si>
+  <si>
+    <t>0xc000506398</t>
   </si>
   <si>
     <t>"09-22-12</t>
   </si>
   <si>
-    <t>0xc0000639c0</t>
-  </si>
-  <si>
-    <t>0xc0000639b0</t>
-  </si>
-  <si>
-    <t>0xc0000639d0</t>
-  </si>
-  <si>
-    <t>0xc0000639e0</t>
-  </si>
-  <si>
-    <t>0xc0000639f0</t>
-  </si>
-  <si>
-    <t>0xc0000246c0</t>
-  </si>
-  <si>
-    <t>0xc0000246d8</t>
+    <t>0xc0005003e0</t>
+  </si>
+  <si>
+    <t>0xc0005003d0</t>
+  </si>
+  <si>
+    <t>0xc0005003f0</t>
+  </si>
+  <si>
+    <t>0xc000500400</t>
+  </si>
+  <si>
+    <t>0xc000500410</t>
+  </si>
+  <si>
+    <t>0xc0005063e0</t>
+  </si>
+  <si>
+    <t>0xc0005063f8</t>
   </si>
   <si>
     <t>"09-22-13</t>
   </si>
   <si>
-    <t>0xc000063a10</t>
-  </si>
-  <si>
-    <t>0xc000063a00</t>
-  </si>
-  <si>
-    <t>0xc000063a20</t>
-  </si>
-  <si>
-    <t>0xc000063a30</t>
-  </si>
-  <si>
-    <t>0xc000063a40</t>
-  </si>
-  <si>
-    <t>0xc000024710</t>
-  </si>
-  <si>
-    <t>0xc000024720</t>
+    <t>0xc000500430</t>
+  </si>
+  <si>
+    <t>0xc000500420</t>
+  </si>
+  <si>
+    <t>0xc000500440</t>
+  </si>
+  <si>
+    <t>0xc000500450</t>
+  </si>
+  <si>
+    <t>0xc000500460</t>
+  </si>
+  <si>
+    <t>0xc000506430</t>
+  </si>
+  <si>
+    <t>0xc000506440</t>
   </si>
   <si>
     <t>"09-22-14</t>
   </si>
   <si>
-    <t>0xc000063a60</t>
-  </si>
-  <si>
-    <t>0xc000063a50</t>
-  </si>
-  <si>
-    <t>0xc000063a70</t>
-  </si>
-  <si>
-    <t>0xc000063a80</t>
-  </si>
-  <si>
-    <t>0xc000063a90</t>
-  </si>
-  <si>
-    <t>0xc000024770</t>
-  </si>
-  <si>
-    <t>0xc000024780</t>
+    <t>0xc000500480</t>
+  </si>
+  <si>
+    <t>0xc000500470</t>
+  </si>
+  <si>
+    <t>0xc000500490</t>
+  </si>
+  <si>
+    <t>0xc0005004a0</t>
+  </si>
+  <si>
+    <t>0xc0005004b0</t>
+  </si>
+  <si>
+    <t>0xc000506490</t>
+  </si>
+  <si>
+    <t>0xc0005064a0</t>
   </si>
   <si>
     <t>"09-22-15</t>
   </si>
   <si>
-    <t>0xc000063ab0</t>
-  </si>
-  <si>
-    <t>0xc000063aa0</t>
-  </si>
-  <si>
-    <t>0xc000063ac0</t>
-  </si>
-  <si>
-    <t>0xc000063ad0</t>
-  </si>
-  <si>
-    <t>0xc000063ae0</t>
-  </si>
-  <si>
-    <t>0xc0000247b0</t>
-  </si>
-  <si>
-    <t>0xc0000247c8</t>
+    <t>0xc0005004d0</t>
+  </si>
+  <si>
+    <t>0xc0005004c0</t>
+  </si>
+  <si>
+    <t>0xc0005004e0</t>
+  </si>
+  <si>
+    <t>0xc0005004f0</t>
+  </si>
+  <si>
+    <t>0xc000500500</t>
+  </si>
+  <si>
+    <t>0xc0005064d0</t>
+  </si>
+  <si>
+    <t>0xc0005064e8</t>
   </si>
   <si>
     <t>"09-22-16</t>
   </si>
   <si>
-    <t>0xc000063b00</t>
-  </si>
-  <si>
-    <t>0xc000063af0</t>
-  </si>
-  <si>
-    <t>0xc000063b10</t>
-  </si>
-  <si>
-    <t>0xc000063b20</t>
-  </si>
-  <si>
-    <t>0xc000063b30</t>
-  </si>
-  <si>
-    <t>0xc000024800</t>
-  </si>
-  <si>
-    <t>0xc000024810</t>
+    <t>0xc000500520</t>
+  </si>
+  <si>
+    <t>0xc000500510</t>
+  </si>
+  <si>
+    <t>0xc000500530</t>
+  </si>
+  <si>
+    <t>0xc000500540</t>
+  </si>
+  <si>
+    <t>0xc000500550</t>
+  </si>
+  <si>
+    <t>0xc000506520</t>
+  </si>
+  <si>
+    <t>0xc000506530</t>
   </si>
   <si>
     <t>"09-22-17</t>
   </si>
   <si>
-    <t>0xc000063b50</t>
-  </si>
-  <si>
-    <t>0xc000063b40</t>
-  </si>
-  <si>
-    <t>0xc000063b60</t>
-  </si>
-  <si>
-    <t>0xc000063b70</t>
-  </si>
-  <si>
-    <t>0xc000063b80</t>
-  </si>
-  <si>
-    <t>0xc000024860</t>
-  </si>
-  <si>
-    <t>0xc000024878</t>
+    <t>0xc000500570</t>
+  </si>
+  <si>
+    <t>0xc000500560</t>
+  </si>
+  <si>
+    <t>0xc000500580</t>
+  </si>
+  <si>
+    <t>0xc000500590</t>
+  </si>
+  <si>
+    <t>0xc0005005a0</t>
+  </si>
+  <si>
+    <t>0xc000506580</t>
+  </si>
+  <si>
+    <t>0xc000506598</t>
   </si>
   <si>
     <t>"09-22-18</t>
   </si>
   <si>
-    <t>0xc000063ba0</t>
-  </si>
-  <si>
-    <t>0xc000063b90</t>
-  </si>
-  <si>
-    <t>0xc000063bb0</t>
-  </si>
-  <si>
-    <t>0xc000063bc0</t>
-  </si>
-  <si>
-    <t>0xc000063bd0</t>
-  </si>
-  <si>
-    <t>0xc0000248b0</t>
-  </si>
-  <si>
-    <t>0xc0000248c0</t>
+    <t>0xc0005005c0</t>
+  </si>
+  <si>
+    <t>0xc0005005b0</t>
+  </si>
+  <si>
+    <t>0xc0005005d0</t>
+  </si>
+  <si>
+    <t>0xc0005005e0</t>
+  </si>
+  <si>
+    <t>0xc0005005f0</t>
+  </si>
+  <si>
+    <t>0xc0005065d0</t>
+  </si>
+  <si>
+    <t>0xc0005065e0</t>
   </si>
   <si>
     <t>"09-22-19</t>
   </si>
   <si>
-    <t>0xc000063bf0</t>
-  </si>
-  <si>
-    <t>0xc000063be0</t>
-  </si>
-  <si>
-    <t>0xc000063c00</t>
-  </si>
-  <si>
-    <t>0xc000063c10</t>
-  </si>
-  <si>
-    <t>0xc000063c20</t>
-  </si>
-  <si>
-    <t>0xc000024900</t>
-  </si>
-  <si>
-    <t>0xc000024910</t>
+    <t>0xc000500610</t>
+  </si>
+  <si>
+    <t>0xc000500600</t>
+  </si>
+  <si>
+    <t>0xc000500620</t>
+  </si>
+  <si>
+    <t>0xc000500630</t>
+  </si>
+  <si>
+    <t>0xc000500640</t>
+  </si>
+  <si>
+    <t>0xc000506620</t>
+  </si>
+  <si>
+    <t>0xc000506630</t>
   </si>
   <si>
     <t>07-22-01</t>
   </si>
   <si>
-    <t>0xc000063c40</t>
+    <t>0xc000500660</t>
   </si>
   <si>
     <t>W</t>
   </si>
   <si>
-    <t>0xc000063c30</t>
-  </si>
-  <si>
-    <t>0xc000063c50</t>
-  </si>
-  <si>
-    <t>0xc000063c60</t>
-  </si>
-  <si>
-    <t>0xc000063c70</t>
-  </si>
-  <si>
-    <t>0xc000024930</t>
+    <t>0xc000500650</t>
+  </si>
+  <si>
+    <t>0xc000500670</t>
+  </si>
+  <si>
+    <t>0xc000500680</t>
+  </si>
+  <si>
+    <t>0xc000500690</t>
+  </si>
+  <si>
+    <t>0xc000506650</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>0xc000024940</t>
+    <t>0xc000506660</t>
   </si>
   <si>
     <t>07-22-02</t>
   </si>
   <si>
-    <t>0xc000063c90</t>
-  </si>
-  <si>
-    <t>0xc000063c80</t>
-  </si>
-  <si>
-    <t>0xc000063ca0</t>
-  </si>
-  <si>
-    <t>0xc000063cb0</t>
-  </si>
-  <si>
-    <t>0xc000063cc0</t>
-  </si>
-  <si>
-    <t>0xc000024950</t>
-  </si>
-  <si>
-    <t>0xc000024960</t>
+    <t>0xc0005006b0</t>
+  </si>
+  <si>
+    <t>0xc0005006a0</t>
+  </si>
+  <si>
+    <t>0xc0005006c0</t>
+  </si>
+  <si>
+    <t>0xc0005006d0</t>
+  </si>
+  <si>
+    <t>0xc0005006e0</t>
+  </si>
+  <si>
+    <t>0xc000506670</t>
+  </si>
+  <si>
+    <t>0xc000506680</t>
   </si>
   <si>
     <t>07-22-03</t>
   </si>
   <si>
-    <t>0xc000063ce0</t>
-  </si>
-  <si>
-    <t>0xc000063cd0</t>
-  </si>
-  <si>
-    <t>0xc000063cf0</t>
-  </si>
-  <si>
-    <t>0xc000063d00</t>
-  </si>
-  <si>
-    <t>0xc000063d10</t>
-  </si>
-  <si>
-    <t>0xc000024970</t>
-  </si>
-  <si>
-    <t>0xc000024980</t>
+    <t>0xc000500700</t>
+  </si>
+  <si>
+    <t>0xc0005006f0</t>
+  </si>
+  <si>
+    <t>0xc000500710</t>
+  </si>
+  <si>
+    <t>0xc000500720</t>
+  </si>
+  <si>
+    <t>0xc000500730</t>
+  </si>
+  <si>
+    <t>0xc000506690</t>
+  </si>
+  <si>
+    <t>0xc0005066a0</t>
   </si>
   <si>
     <t>07-22-04</t>
   </si>
   <si>
-    <t>0xc000063d30</t>
-  </si>
-  <si>
-    <t>0xc000063d20</t>
-  </si>
-  <si>
-    <t>0xc000063d40</t>
-  </si>
-  <si>
-    <t>0xc000063d50</t>
-  </si>
-  <si>
-    <t>0xc000063d60</t>
-  </si>
-  <si>
-    <t>0xc0000249a0</t>
-  </si>
-  <si>
-    <t>0xc0000249b0</t>
+    <t>0xc000500750</t>
+  </si>
+  <si>
+    <t>0xc000500740</t>
+  </si>
+  <si>
+    <t>0xc000500760</t>
+  </si>
+  <si>
+    <t>0xc000500770</t>
+  </si>
+  <si>
+    <t>0xc000500780</t>
+  </si>
+  <si>
+    <t>0xc0005066c0</t>
+  </si>
+  <si>
+    <t>0xc0005066d0</t>
   </si>
   <si>
     <t>07-22-05</t>
   </si>
   <si>
-    <t>0xc000063d80</t>
-  </si>
-  <si>
-    <t>0xc000063d70</t>
-  </si>
-  <si>
-    <t>0xc000063d90</t>
-  </si>
-  <si>
-    <t>0xc000063da0</t>
-  </si>
-  <si>
-    <t>0xc000063db0</t>
-  </si>
-  <si>
-    <t>0xc0000249c0</t>
-  </si>
-  <si>
-    <t>0xc0000249d0</t>
+    <t>0xc0005007a0</t>
+  </si>
+  <si>
+    <t>0xc000500790</t>
+  </si>
+  <si>
+    <t>0xc0005007b0</t>
+  </si>
+  <si>
+    <t>0xc0005007c0</t>
+  </si>
+  <si>
+    <t>0xc0005007d0</t>
+  </si>
+  <si>
+    <t>0xc0005066e0</t>
+  </si>
+  <si>
+    <t>0xc0005066f0</t>
   </si>
   <si>
     <t>07-22-06</t>
   </si>
   <si>
-    <t>0xc000063dd0</t>
-  </si>
-  <si>
-    <t>0xc000063dc0</t>
-  </si>
-  <si>
-    <t>0xc000063de0</t>
-  </si>
-  <si>
-    <t>0xc000063df0</t>
-  </si>
-  <si>
-    <t>0xc000063e00</t>
-  </si>
-  <si>
-    <t>0xc0000249f0</t>
-  </si>
-  <si>
-    <t>0xc000024a00</t>
+    <t>0xc0005007f0</t>
+  </si>
+  <si>
+    <t>0xc0005007e0</t>
+  </si>
+  <si>
+    <t>0xc000500800</t>
+  </si>
+  <si>
+    <t>0xc000500810</t>
+  </si>
+  <si>
+    <t>0xc000500820</t>
+  </si>
+  <si>
+    <t>0xc000506710</t>
+  </si>
+  <si>
+    <t>0xc000506720</t>
   </si>
   <si>
     <t>07-22-07</t>
   </si>
   <si>
-    <t>0xc000063e20</t>
-  </si>
-  <si>
-    <t>0xc000063e10</t>
-  </si>
-  <si>
-    <t>0xc000063e30</t>
-  </si>
-  <si>
-    <t>0xc000063e40</t>
-  </si>
-  <si>
-    <t>0xc000063e50</t>
-  </si>
-  <si>
-    <t>0xc000024a20</t>
-  </si>
-  <si>
-    <t>0xc000024a30</t>
+    <t>0xc000500840</t>
+  </si>
+  <si>
+    <t>0xc000500830</t>
+  </si>
+  <si>
+    <t>0xc000500850</t>
+  </si>
+  <si>
+    <t>0xc000500860</t>
+  </si>
+  <si>
+    <t>0xc000500870</t>
+  </si>
+  <si>
+    <t>0xc000506740</t>
+  </si>
+  <si>
+    <t>0xc000506750</t>
   </si>
   <si>
     <t>07-22-08</t>
   </si>
   <si>
-    <t>0xc000063e70</t>
-  </si>
-  <si>
-    <t>0xc000063e60</t>
-  </si>
-  <si>
-    <t>0xc000063e80</t>
-  </si>
-  <si>
-    <t>0xc000063e90</t>
-  </si>
-  <si>
-    <t>0xc000063ea0</t>
-  </si>
-  <si>
-    <t>0xc000024a60</t>
-  </si>
-  <si>
-    <t>0xc000024a70</t>
+    <t>0xc000500890</t>
+  </si>
+  <si>
+    <t>0xc000500880</t>
+  </si>
+  <si>
+    <t>0xc0005008a0</t>
+  </si>
+  <si>
+    <t>0xc0005008b0</t>
+  </si>
+  <si>
+    <t>0xc0005008c0</t>
+  </si>
+  <si>
+    <t>0xc000506780</t>
+  </si>
+  <si>
+    <t>0xc000506790</t>
   </si>
   <si>
     <t>07-22-09</t>
   </si>
   <si>
-    <t>0xc000063ec0</t>
-  </si>
-  <si>
-    <t>0xc000063eb0</t>
-  </si>
-  <si>
-    <t>0xc000063ed0</t>
-  </si>
-  <si>
-    <t>0xc000063ee0</t>
-  </si>
-  <si>
-    <t>0xc000063ef0</t>
-  </si>
-  <si>
-    <t>0xc000024a90</t>
-  </si>
-  <si>
-    <t>0xc000024aa0</t>
+    <t>0xc0005008e0</t>
+  </si>
+  <si>
+    <t>0xc0005008d0</t>
+  </si>
+  <si>
+    <t>0xc0005008f0</t>
+  </si>
+  <si>
+    <t>0xc000500900</t>
+  </si>
+  <si>
+    <t>0xc000500910</t>
+  </si>
+  <si>
+    <t>0xc0005067b0</t>
+  </si>
+  <si>
+    <t>0xc0005067c0</t>
   </si>
   <si>
     <t>07-22-10</t>
   </si>
   <si>
-    <t>0xc000063f10</t>
-  </si>
-  <si>
-    <t>0xc000063f00</t>
-  </si>
-  <si>
-    <t>0xc000063f20</t>
-  </si>
-  <si>
-    <t>0xc000063f30</t>
-  </si>
-  <si>
-    <t>0xc000063f40</t>
-  </si>
-  <si>
-    <t>0xc000024ad0</t>
-  </si>
-  <si>
-    <t>0xc000024ae0</t>
+    <t>0xc000500930</t>
+  </si>
+  <si>
+    <t>0xc000500920</t>
+  </si>
+  <si>
+    <t>0xc000500940</t>
+  </si>
+  <si>
+    <t>0xc000500950</t>
+  </si>
+  <si>
+    <t>0xc000500960</t>
+  </si>
+  <si>
+    <t>0xc0005067f0</t>
+  </si>
+  <si>
+    <t>0xc000506800</t>
   </si>
   <si>
     <t>07-22-11</t>
   </si>
   <si>
-    <t>0xc000063f60</t>
-  </si>
-  <si>
-    <t>0xc000063f50</t>
-  </si>
-  <si>
-    <t>0xc000063f70</t>
-  </si>
-  <si>
-    <t>0xc000063f80</t>
-  </si>
-  <si>
-    <t>0xc000063f90</t>
-  </si>
-  <si>
-    <t>0xc000024b10</t>
-  </si>
-  <si>
-    <t>0xc000024b40</t>
+    <t>0xc000500980</t>
+  </si>
+  <si>
+    <t>0xc000500970</t>
+  </si>
+  <si>
+    <t>0xc000500990</t>
+  </si>
+  <si>
+    <t>0xc0005009a0</t>
+  </si>
+  <si>
+    <t>0xc0005009b0</t>
+  </si>
+  <si>
+    <t>0xc000506830</t>
+  </si>
+  <si>
+    <t>0xc000506840</t>
   </si>
   <si>
     <t>07-22-12</t>
   </si>
   <si>
-    <t>0xc000063fb0</t>
-  </si>
-  <si>
-    <t>0xc000063fa0</t>
-  </si>
-  <si>
-    <t>0xc000063fc0</t>
-  </si>
-  <si>
-    <t>0xc000063fd0</t>
-  </si>
-  <si>
-    <t>0xc000063fe0</t>
-  </si>
-  <si>
-    <t>0xc000024bd0</t>
-  </si>
-  <si>
-    <t>0xc000024be0</t>
+    <t>0xc0005009d0</t>
+  </si>
+  <si>
+    <t>0xc0005009c0</t>
+  </si>
+  <si>
+    <t>0xc0005009e0</t>
+  </si>
+  <si>
+    <t>0xc0005009f0</t>
+  </si>
+  <si>
+    <t>0xc000500a00</t>
+  </si>
+  <si>
+    <t>0xc000506870</t>
+  </si>
+  <si>
+    <t>0xc000506880</t>
   </si>
   <si>
     <t>07-22-13</t>
   </si>
   <si>
-    <t>0xc00039e000</t>
-  </si>
-  <si>
-    <t>0xc000063ff0</t>
-  </si>
-  <si>
-    <t>0xc00039e010</t>
-  </si>
-  <si>
-    <t>0xc00039e020</t>
-  </si>
-  <si>
-    <t>0xc00039e030</t>
-  </si>
-  <si>
-    <t>0xc000024c00</t>
-  </si>
-  <si>
-    <t>0xc000024c10</t>
+    <t>0xc000500a20</t>
+  </si>
+  <si>
+    <t>0xc000500a10</t>
+  </si>
+  <si>
+    <t>0xc000500a30</t>
+  </si>
+  <si>
+    <t>0xc000500a40</t>
+  </si>
+  <si>
+    <t>0xc000500a50</t>
+  </si>
+  <si>
+    <t>0xc0005068a0</t>
+  </si>
+  <si>
+    <t>0xc0005068b0</t>
   </si>
   <si>
     <t>07-22-14</t>
   </si>
   <si>
-    <t>0xc00039e050</t>
-  </si>
-  <si>
-    <t>0xc00039e040</t>
-  </si>
-  <si>
-    <t>0xc00039e060</t>
-  </si>
-  <si>
-    <t>0xc00039e070</t>
-  </si>
-  <si>
-    <t>0xc00039e080</t>
-  </si>
-  <si>
-    <t>0xc000024c40</t>
-  </si>
-  <si>
-    <t>0xc000024c50</t>
+    <t>0xc000500a70</t>
+  </si>
+  <si>
+    <t>0xc000500a60</t>
+  </si>
+  <si>
+    <t>0xc000500a80</t>
+  </si>
+  <si>
+    <t>0xc000500a90</t>
+  </si>
+  <si>
+    <t>0xc000500aa0</t>
+  </si>
+  <si>
+    <t>0xc0005068e0</t>
+  </si>
+  <si>
+    <t>0xc0005068f0</t>
   </si>
   <si>
     <t>07-22-15</t>
   </si>
   <si>
-    <t>0xc00039e0a0</t>
-  </si>
-  <si>
-    <t>0xc00039e090</t>
-  </si>
-  <si>
-    <t>0xc00039e0b0</t>
-  </si>
-  <si>
-    <t>0xc00039e0c0</t>
-  </si>
-  <si>
-    <t>0xc00039e0d0</t>
-  </si>
-  <si>
-    <t>0xc000024c70</t>
-  </si>
-  <si>
-    <t>0xc000024c80</t>
+    <t>0xc000500ac0</t>
+  </si>
+  <si>
+    <t>0xc000500ab0</t>
+  </si>
+  <si>
+    <t>0xc000500ad0</t>
+  </si>
+  <si>
+    <t>0xc000500ae0</t>
+  </si>
+  <si>
+    <t>0xc000500af0</t>
+  </si>
+  <si>
+    <t>0xc000506910</t>
+  </si>
+  <si>
+    <t>0xc000506920</t>
   </si>
   <si>
     <t>07-22-16</t>
   </si>
   <si>
-    <t>0xc00039e0f0</t>
-  </si>
-  <si>
-    <t>0xc00039e0e0</t>
-  </si>
-  <si>
-    <t>0xc00039e100</t>
-  </si>
-  <si>
-    <t>0xc00039e110</t>
-  </si>
-  <si>
-    <t>0xc00039e120</t>
-  </si>
-  <si>
-    <t>0xc000024ca0</t>
-  </si>
-  <si>
-    <t>0xc000024cb0</t>
+    <t>0xc000500b10</t>
+  </si>
+  <si>
+    <t>0xc000500b00</t>
+  </si>
+  <si>
+    <t>0xc000500b20</t>
+  </si>
+  <si>
+    <t>0xc000500b30</t>
+  </si>
+  <si>
+    <t>0xc000500b40</t>
+  </si>
+  <si>
+    <t>0xc000506940</t>
+  </si>
+  <si>
+    <t>0xc000506950</t>
   </si>
   <si>
     <t>07-22-17</t>
   </si>
   <si>
-    <t>0xc00039e140</t>
-  </si>
-  <si>
-    <t>0xc00039e130</t>
-  </si>
-  <si>
-    <t>0xc00039e150</t>
-  </si>
-  <si>
-    <t>0xc00039e160</t>
-  </si>
-  <si>
-    <t>0xc00039e170</t>
-  </si>
-  <si>
-    <t>0xc000024ce0</t>
-  </si>
-  <si>
-    <t>0xc000024cf0</t>
+    <t>0xc000500b60</t>
+  </si>
+  <si>
+    <t>0xc000500b50</t>
+  </si>
+  <si>
+    <t>0xc000500ba0</t>
+  </si>
+  <si>
+    <t>0xc000500c00</t>
+  </si>
+  <si>
+    <t>0xc000500c10</t>
+  </si>
+  <si>
+    <t>0xc000506980</t>
+  </si>
+  <si>
+    <t>0xc000506990</t>
   </si>
   <si>
     <t>07-22-18</t>
   </si>
   <si>
-    <t>0xc00039e190</t>
-  </si>
-  <si>
-    <t>0xc00039e180</t>
-  </si>
-  <si>
-    <t>0xc00039e1a0</t>
-  </si>
-  <si>
-    <t>0xc00039e1b0</t>
-  </si>
-  <si>
-    <t>0xc00039e1c0</t>
-  </si>
-  <si>
-    <t>0xc000024d20</t>
-  </si>
-  <si>
-    <t>0xc000024d30</t>
+    <t>0xc000500c40</t>
+  </si>
+  <si>
+    <t>0xc000500c30</t>
+  </si>
+  <si>
+    <t>0xc000500c50</t>
+  </si>
+  <si>
+    <t>0xc000500c60</t>
+  </si>
+  <si>
+    <t>0xc000500c70</t>
+  </si>
+  <si>
+    <t>0xc0005069c0</t>
+  </si>
+  <si>
+    <t>0xc0005069d0</t>
   </si>
   <si>
     <t>07-22-19</t>
   </si>
   <si>
-    <t>0xc00039e1e0</t>
-  </si>
-  <si>
-    <t>0xc00039e1d0</t>
-  </si>
-  <si>
-    <t>0xc00039e1f0</t>
-  </si>
-  <si>
-    <t>0xc00039e200</t>
-  </si>
-  <si>
-    <t>0xc00039e210</t>
-  </si>
-  <si>
-    <t>0xc000024d50</t>
-  </si>
-  <si>
-    <t>0xc000024d60</t>
+    <t>0xc000500c90</t>
+  </si>
+  <si>
+    <t>0xc000500c80</t>
+  </si>
+  <si>
+    <t>0xc000500ca0</t>
+  </si>
+  <si>
+    <t>0xc000500cb0</t>
+  </si>
+  <si>
+    <t>0xc000500cc0</t>
+  </si>
+  <si>
+    <t>0xc0005069f0</t>
+  </si>
+  <si>
+    <t>0xc000506a00</t>
   </si>
   <si>
     <t>07-22-20</t>
   </si>
   <si>
-    <t>0xc00039e230</t>
-  </si>
-  <si>
-    <t>0xc00039e220</t>
-  </si>
-  <si>
-    <t>0xc00039e240</t>
-  </si>
-  <si>
-    <t>0xc00039e250</t>
-  </si>
-  <si>
-    <t>0xc00039e260</t>
-  </si>
-  <si>
-    <t>0xc000024d90</t>
-  </si>
-  <si>
-    <t>0xc000024da0</t>
+    <t>0xc000500ce0</t>
+  </si>
+  <si>
+    <t>0xc000500cd0</t>
+  </si>
+  <si>
+    <t>0xc000500cf0</t>
+  </si>
+  <si>
+    <t>0xc000500d00</t>
+  </si>
+  <si>
+    <t>0xc000500d10</t>
+  </si>
+  <si>
+    <t>0xc000506a30</t>
+  </si>
+  <si>
+    <t>0xc000506a40</t>
   </si>
   <si>
     <t>07-22-21</t>
   </si>
   <si>
-    <t>0xc00039e280</t>
-  </si>
-  <si>
-    <t>0xc00039e270</t>
-  </si>
-  <si>
-    <t>0xc00039e290</t>
-  </si>
-  <si>
-    <t>0xc00039e2a0</t>
-  </si>
-  <si>
-    <t>0xc00039e2b0</t>
-  </si>
-  <si>
-    <t>0xc000024dd0</t>
-  </si>
-  <si>
-    <t>0xc000024de0</t>
+    <t>0xc000500d30</t>
+  </si>
+  <si>
+    <t>0xc000500d20</t>
+  </si>
+  <si>
+    <t>0xc000500d40</t>
+  </si>
+  <si>
+    <t>0xc000500d50</t>
+  </si>
+  <si>
+    <t>0xc000500d60</t>
+  </si>
+  <si>
+    <t>0xc000506a70</t>
+  </si>
+  <si>
+    <t>0xc000506a80</t>
   </si>
   <si>
     <t>08-22-01</t>
   </si>
   <si>
-    <t>0xc00039e2d0</t>
-  </si>
-  <si>
-    <t>0xc00039e2c0</t>
-  </si>
-  <si>
-    <t>0xc00039e2e0</t>
-  </si>
-  <si>
-    <t>0xc00039e2f0</t>
-  </si>
-  <si>
-    <t>0xc00039e300</t>
-  </si>
-  <si>
-    <t>0xc000024e00</t>
-  </si>
-  <si>
-    <t>0xc000024e10</t>
+    <t>0xc000500d80</t>
+  </si>
+  <si>
+    <t>0xc000500d70</t>
+  </si>
+  <si>
+    <t>0xc000500d90</t>
+  </si>
+  <si>
+    <t>0xc000500da0</t>
+  </si>
+  <si>
+    <t>0xc000500db0</t>
+  </si>
+  <si>
+    <t>0xc000506aa0</t>
+  </si>
+  <si>
+    <t>0xc000506ab0</t>
   </si>
   <si>
     <t>08-22-02</t>
   </si>
   <si>
-    <t>0xc00039e320</t>
-  </si>
-  <si>
-    <t>0xc00039e310</t>
-  </si>
-  <si>
-    <t>0xc00039e330</t>
-  </si>
-  <si>
-    <t>0xc00039e340</t>
-  </si>
-  <si>
-    <t>0xc00039e350</t>
-  </si>
-  <si>
-    <t>0xc000024e30</t>
-  </si>
-  <si>
-    <t>0xc000024e40</t>
+    <t>0xc000500dd0</t>
+  </si>
+  <si>
+    <t>0xc000500dc0</t>
+  </si>
+  <si>
+    <t>0xc000500de0</t>
+  </si>
+  <si>
+    <t>0xc000500df0</t>
+  </si>
+  <si>
+    <t>0xc000500e00</t>
+  </si>
+  <si>
+    <t>0xc000506ad0</t>
+  </si>
+  <si>
+    <t>0xc000506ae0</t>
   </si>
   <si>
     <t>08-22-03</t>
   </si>
   <si>
-    <t>0xc00039e370</t>
-  </si>
-  <si>
-    <t>0xc00039e360</t>
-  </si>
-  <si>
-    <t>0xc00039e380</t>
-  </si>
-  <si>
-    <t>0xc00039e390</t>
-  </si>
-  <si>
-    <t>0xc00039e3a0</t>
-  </si>
-  <si>
-    <t>0xc000024e58</t>
-  </si>
-  <si>
-    <t>0xc000024e68</t>
+    <t>0xc000500e20</t>
+  </si>
+  <si>
+    <t>0xc000500e10</t>
+  </si>
+  <si>
+    <t>0xc000500e30</t>
+  </si>
+  <si>
+    <t>0xc000500e40</t>
+  </si>
+  <si>
+    <t>0xc000500e50</t>
+  </si>
+  <si>
+    <t>0xc000506af8</t>
+  </si>
+  <si>
+    <t>0xc000506b08</t>
   </si>
   <si>
     <t>08-22-04</t>
   </si>
   <si>
-    <t>0xc00039e3c0</t>
-  </si>
-  <si>
-    <t>0xc00039e3b0</t>
-  </si>
-  <si>
-    <t>0xc00039e3d0</t>
-  </si>
-  <si>
-    <t>0xc00039e3e0</t>
-  </si>
-  <si>
-    <t>0xc00039e3f0</t>
-  </si>
-  <si>
-    <t>0xc000024ea0</t>
-  </si>
-  <si>
-    <t>0xc000024ec0</t>
+    <t>0xc000500e70</t>
+  </si>
+  <si>
+    <t>0xc000500e60</t>
+  </si>
+  <si>
+    <t>0xc000500e80</t>
+  </si>
+  <si>
+    <t>0xc000500e90</t>
+  </si>
+  <si>
+    <t>0xc000500ea0</t>
+  </si>
+  <si>
+    <t>0xc000506b30</t>
+  </si>
+  <si>
+    <t>0xc000506b40</t>
   </si>
   <si>
     <t>08-22-05</t>
   </si>
   <si>
-    <t>0xc00039e410</t>
-  </si>
-  <si>
-    <t>0xc00039e400</t>
-  </si>
-  <si>
-    <t>0xc00039e420</t>
-  </si>
-  <si>
-    <t>0xc00039e430</t>
-  </si>
-  <si>
-    <t>0xc00039e440</t>
-  </si>
-  <si>
-    <t>0xc000024ed8</t>
-  </si>
-  <si>
-    <t>0xc000024ef8</t>
+    <t>0xc000500ec0</t>
+  </si>
+  <si>
+    <t>0xc000500eb0</t>
+  </si>
+  <si>
+    <t>0xc000500ed0</t>
+  </si>
+  <si>
+    <t>0xc000500ee0</t>
+  </si>
+  <si>
+    <t>0xc000500ef0</t>
+  </si>
+  <si>
+    <t>0xc000506b58</t>
+  </si>
+  <si>
+    <t>0xc000506b68</t>
   </si>
   <si>
     <t>08-22-06</t>
   </si>
   <si>
-    <t>0xc00039e460</t>
-  </si>
-  <si>
-    <t>0xc00039e450</t>
-  </si>
-  <si>
-    <t>0xc00039e470</t>
-  </si>
-  <si>
-    <t>0xc00039e480</t>
-  </si>
-  <si>
-    <t>0xc00039e490</t>
-  </si>
-  <si>
-    <t>0xc000024f30</t>
-  </si>
-  <si>
-    <t>0xc000024f60</t>
+    <t>0xc000500f10</t>
+  </si>
+  <si>
+    <t>0xc000500f00</t>
+  </si>
+  <si>
+    <t>0xc000500f20</t>
+  </si>
+  <si>
+    <t>0xc000500f30</t>
+  </si>
+  <si>
+    <t>0xc000500f40</t>
+  </si>
+  <si>
+    <t>0xc000506b80</t>
+  </si>
+  <si>
+    <t>0xc000506b90</t>
   </si>
   <si>
     <t>08-22-07</t>
   </si>
   <si>
-    <t>0xc00039e4b0</t>
-  </si>
-  <si>
-    <t>0xc00039e4a0</t>
-  </si>
-  <si>
-    <t>0xc00039e4c0</t>
-  </si>
-  <si>
-    <t>0xc00039e4d0</t>
-  </si>
-  <si>
-    <t>0xc00039e4e0</t>
-  </si>
-  <si>
-    <t>0xc000024fa0</t>
-  </si>
-  <si>
-    <t>0xc000024fc0</t>
+    <t>0xc000500f60</t>
+  </si>
+  <si>
+    <t>0xc000500f50</t>
+  </si>
+  <si>
+    <t>0xc000500f70</t>
+  </si>
+  <si>
+    <t>0xc000500f80</t>
+  </si>
+  <si>
+    <t>0xc000500f90</t>
+  </si>
+  <si>
+    <t>0xc000506bb0</t>
+  </si>
+  <si>
+    <t>0xc000506bc0</t>
   </si>
   <si>
     <t>08-22-08</t>
   </si>
   <si>
-    <t>0xc00039e500</t>
-  </si>
-  <si>
-    <t>0xc00039e4f0</t>
-  </si>
-  <si>
-    <t>0xc00039e510</t>
-  </si>
-  <si>
-    <t>0xc00039e520</t>
-  </si>
-  <si>
-    <t>0xc00039e530</t>
-  </si>
-  <si>
-    <t>0xc000024ff0</t>
-  </si>
-  <si>
-    <t>0xc000025000</t>
+    <t>0xc000500fb0</t>
+  </si>
+  <si>
+    <t>0xc000500fa0</t>
+  </si>
+  <si>
+    <t>0xc000500fc0</t>
+  </si>
+  <si>
+    <t>0xc000500fd0</t>
+  </si>
+  <si>
+    <t>0xc000500fe0</t>
+  </si>
+  <si>
+    <t>0xc000506be0</t>
+  </si>
+  <si>
+    <t>0xc000506bf0</t>
   </si>
   <si>
     <t>08-22-09</t>
   </si>
   <si>
-    <t>0xc00039e550</t>
-  </si>
-  <si>
-    <t>0xc00039e540</t>
-  </si>
-  <si>
-    <t>0xc00039e560</t>
-  </si>
-  <si>
-    <t>0xc00039e570</t>
-  </si>
-  <si>
-    <t>0xc00039e580</t>
-  </si>
-  <si>
-    <t>0xc000025030</t>
-  </si>
-  <si>
-    <t>0xc000025050</t>
+    <t>0xc000501000</t>
+  </si>
+  <si>
+    <t>0xc000500ff0</t>
+  </si>
+  <si>
+    <t>0xc000501010</t>
+  </si>
+  <si>
+    <t>0xc000501020</t>
+  </si>
+  <si>
+    <t>0xc000501030</t>
+  </si>
+  <si>
+    <t>0xc000506c10</t>
+  </si>
+  <si>
+    <t>0xc000506c20</t>
   </si>
   <si>
     <t>08-22-10</t>
   </si>
   <si>
-    <t>0xc00039e5a0</t>
-  </si>
-  <si>
-    <t>0xc00039e590</t>
-  </si>
-  <si>
-    <t>0xc00039e5b0</t>
-  </si>
-  <si>
-    <t>0xc00039e5c0</t>
-  </si>
-  <si>
-    <t>0xc00039e5d0</t>
-  </si>
-  <si>
-    <t>0xc000025080</t>
-  </si>
-  <si>
-    <t>0xc000025090</t>
+    <t>0xc000501050</t>
+  </si>
+  <si>
+    <t>0xc000501040</t>
+  </si>
+  <si>
+    <t>0xc000501060</t>
+  </si>
+  <si>
+    <t>0xc000501070</t>
+  </si>
+  <si>
+    <t>0xc000501080</t>
+  </si>
+  <si>
+    <t>0xc000506c40</t>
+  </si>
+  <si>
+    <t>0xc000506c50</t>
   </si>
   <si>
     <t>08-22-11</t>
   </si>
   <si>
-    <t>0xc00039e5f0</t>
-  </si>
-  <si>
-    <t>0xc00039e5e0</t>
-  </si>
-  <si>
-    <t>0xc00039e600</t>
-  </si>
-  <si>
-    <t>0xc00039e610</t>
-  </si>
-  <si>
-    <t>0xc00039e620</t>
-  </si>
-  <si>
-    <t>0xc0000250b0</t>
-  </si>
-  <si>
-    <t>0xc0000250c0</t>
+    <t>0xc0005010a0</t>
+  </si>
+  <si>
+    <t>0xc000501090</t>
+  </si>
+  <si>
+    <t>0xc0005010b0</t>
+  </si>
+  <si>
+    <t>0xc0005010c0</t>
+  </si>
+  <si>
+    <t>0xc0005010d0</t>
+  </si>
+  <si>
+    <t>0xc000506c70</t>
+  </si>
+  <si>
+    <t>0xc000506c80</t>
   </si>
   <si>
     <t>08-22-12</t>
   </si>
   <si>
-    <t>0xc00039e640</t>
-  </si>
-  <si>
-    <t>0xc00039e630</t>
-  </si>
-  <si>
-    <t>0xc00039e650</t>
-  </si>
-  <si>
-    <t>0xc00039e660</t>
-  </si>
-  <si>
-    <t>0xc00039e670</t>
-  </si>
-  <si>
-    <t>0xc0000250e0</t>
-  </si>
-  <si>
-    <t>0xc0000250f0</t>
+    <t>0xc0005010f0</t>
+  </si>
+  <si>
+    <t>0xc0005010e0</t>
+  </si>
+  <si>
+    <t>0xc000501100</t>
+  </si>
+  <si>
+    <t>0xc000501110</t>
+  </si>
+  <si>
+    <t>0xc000501120</t>
+  </si>
+  <si>
+    <t>0xc000506ca0</t>
+  </si>
+  <si>
+    <t>0xc000506cb0</t>
   </si>
   <si>
     <t>08-22-13</t>
   </si>
   <si>
-    <t>0xc00039e690</t>
-  </si>
-  <si>
-    <t>0xc00039e680</t>
-  </si>
-  <si>
-    <t>0xc00039e6a0</t>
-  </si>
-  <si>
-    <t>0xc00039e6b0</t>
-  </si>
-  <si>
-    <t>0xc00039e6c0</t>
-  </si>
-  <si>
-    <t>0xc000025110</t>
-  </si>
-  <si>
-    <t>0xc000025120</t>
+    <t>0xc000501140</t>
+  </si>
+  <si>
+    <t>0xc000501130</t>
+  </si>
+  <si>
+    <t>0xc000501150</t>
+  </si>
+  <si>
+    <t>0xc000501160</t>
+  </si>
+  <si>
+    <t>0xc000501170</t>
+  </si>
+  <si>
+    <t>0xc000506cd0</t>
+  </si>
+  <si>
+    <t>0xc000506ce0</t>
   </si>
   <si>
     <t>08-22-14</t>
   </si>
   <si>
-    <t>0xc00039e6e0</t>
-  </si>
-  <si>
-    <t>0xc00039e6d0</t>
-  </si>
-  <si>
-    <t>0xc00039e6f0</t>
-  </si>
-  <si>
-    <t>0xc00039e700</t>
-  </si>
-  <si>
-    <t>0xc00039e710</t>
-  </si>
-  <si>
-    <t>0xc000025140</t>
-  </si>
-  <si>
-    <t>0xc000025150</t>
+    <t>0xc000501190</t>
+  </si>
+  <si>
+    <t>0xc000501180</t>
+  </si>
+  <si>
+    <t>0xc0005011a0</t>
+  </si>
+  <si>
+    <t>0xc0005011b0</t>
+  </si>
+  <si>
+    <t>0xc0005011c0</t>
+  </si>
+  <si>
+    <t>0xc000506d00</t>
+  </si>
+  <si>
+    <t>0xc000506d10</t>
   </si>
   <si>
     <t>08-22-15</t>
   </si>
   <si>
-    <t>0xc00039e730</t>
-  </si>
-  <si>
-    <t>0xc00039e720</t>
-  </si>
-  <si>
-    <t>0xc00039e740</t>
-  </si>
-  <si>
-    <t>0xc00039e750</t>
-  </si>
-  <si>
-    <t>0xc00039e760</t>
-  </si>
-  <si>
-    <t>0xc000025170</t>
-  </si>
-  <si>
-    <t>0xc000025180</t>
+    <t>0xc0005011e0</t>
+  </si>
+  <si>
+    <t>0xc0005011d0</t>
+  </si>
+  <si>
+    <t>0xc0005011f0</t>
+  </si>
+  <si>
+    <t>0xc000501200</t>
+  </si>
+  <si>
+    <t>0xc000501210</t>
+  </si>
+  <si>
+    <t>0xc000506d30</t>
+  </si>
+  <si>
+    <t>0xc000506d40</t>
   </si>
   <si>
     <t>08-22-16</t>
   </si>
   <si>
-    <t>0xc00039e780</t>
-  </si>
-  <si>
-    <t>0xc00039e770</t>
-  </si>
-  <si>
-    <t>0xc00039e790</t>
-  </si>
-  <si>
-    <t>0xc00039e7a0</t>
-  </si>
-  <si>
-    <t>0xc00039e7b0</t>
-  </si>
-  <si>
-    <t>0xc0000251a0</t>
-  </si>
-  <si>
-    <t>0xc0000251b0</t>
+    <t>0xc000501230</t>
+  </si>
+  <si>
+    <t>0xc000501220</t>
+  </si>
+  <si>
+    <t>0xc000501240</t>
+  </si>
+  <si>
+    <t>0xc000501250</t>
+  </si>
+  <si>
+    <t>0xc000501260</t>
+  </si>
+  <si>
+    <t>0xc000506d60</t>
+  </si>
+  <si>
+    <t>0xc000506d70</t>
   </si>
   <si>
     <t>08-22-17</t>
   </si>
   <si>
-    <t>0xc00039e7d0</t>
-  </si>
-  <si>
-    <t>0xc00039e7c0</t>
-  </si>
-  <si>
-    <t>0xc00039e7e0</t>
-  </si>
-  <si>
-    <t>0xc00039e7f0</t>
-  </si>
-  <si>
-    <t>0xc00039e800</t>
-  </si>
-  <si>
-    <t>0xc0000251d0</t>
-  </si>
-  <si>
-    <t>0xc0000251e0</t>
+    <t>0xc000501280</t>
+  </si>
+  <si>
+    <t>0xc000501270</t>
+  </si>
+  <si>
+    <t>0xc000501290</t>
+  </si>
+  <si>
+    <t>0xc0005012a0</t>
+  </si>
+  <si>
+    <t>0xc0005012b0</t>
+  </si>
+  <si>
+    <t>0xc000506d90</t>
+  </si>
+  <si>
+    <t>0xc000506da0</t>
   </si>
   <si>
     <t>08-22-18</t>
   </si>
   <si>
-    <t>0xc00039e820</t>
-  </si>
-  <si>
-    <t>0xc00039e810</t>
-  </si>
-  <si>
-    <t>0xc00039e830</t>
-  </si>
-  <si>
-    <t>0xc00039e840</t>
-  </si>
-  <si>
-    <t>0xc00039e850</t>
-  </si>
-  <si>
-    <t>0xc0000251f8</t>
-  </si>
-  <si>
-    <t>0xc000025218</t>
+    <t>0xc0005012d0</t>
+  </si>
+  <si>
+    <t>0xc0005012c0</t>
+  </si>
+  <si>
+    <t>0xc0005012e0</t>
+  </si>
+  <si>
+    <t>0xc0005012f0</t>
+  </si>
+  <si>
+    <t>0xc000501300</t>
+  </si>
+  <si>
+    <t>0xc000506db8</t>
+  </si>
+  <si>
+    <t>0xc000506dd8</t>
   </si>
   <si>
     <t>08-22-19</t>
   </si>
   <si>
-    <t>0xc00039e870</t>
-  </si>
-  <si>
-    <t>0xc00039e860</t>
-  </si>
-  <si>
-    <t>0xc00039e880</t>
-  </si>
-  <si>
-    <t>0xc00039e890</t>
-  </si>
-  <si>
-    <t>0xc00039e8a0</t>
-  </si>
-  <si>
-    <t>0xc000025240</t>
-  </si>
-  <si>
-    <t>0xc000025250</t>
+    <t>0xc000501320</t>
+  </si>
+  <si>
+    <t>0xc000501310</t>
+  </si>
+  <si>
+    <t>0xc000501330</t>
+  </si>
+  <si>
+    <t>0xc000501340</t>
+  </si>
+  <si>
+    <t>0xc000501350</t>
+  </si>
+  <si>
+    <t>0xc000506e00</t>
+  </si>
+  <si>
+    <t>0xc000506e10</t>
   </si>
   <si>
     <t>08-22-20</t>
   </si>
   <si>
-    <t>0xc00039e8c0</t>
-  </si>
-  <si>
-    <t>0xc00039e8b0</t>
-  </si>
-  <si>
-    <t>0xc00039e8d0</t>
-  </si>
-  <si>
-    <t>0xc00039e8e0</t>
-  </si>
-  <si>
-    <t>0xc00039e8f0</t>
-  </si>
-  <si>
-    <t>0xc000025270</t>
-  </si>
-  <si>
-    <t>0xc000025280</t>
+    <t>0xc000501370</t>
+  </si>
+  <si>
+    <t>0xc000501360</t>
+  </si>
+  <si>
+    <t>0xc000501380</t>
+  </si>
+  <si>
+    <t>0xc000501390</t>
+  </si>
+  <si>
+    <t>0xc0005013a0</t>
+  </si>
+  <si>
+    <t>0xc000506e30</t>
+  </si>
+  <si>
+    <t>0xc000506e40</t>
   </si>
   <si>
     <t>08-22-21</t>
   </si>
   <si>
-    <t>0xc00039e910</t>
-  </si>
-  <si>
-    <t>0xc00039e900</t>
-  </si>
-  <si>
-    <t>0xc00039e920</t>
-  </si>
-  <si>
-    <t>0xc00039e930</t>
-  </si>
-  <si>
-    <t>0xc00039e940</t>
-  </si>
-  <si>
-    <t>0xc000025298</t>
-  </si>
-  <si>
-    <t>0xc0000252a8</t>
+    <t>0xc0005013c0</t>
+  </si>
+  <si>
+    <t>0xc0005013b0</t>
+  </si>
+  <si>
+    <t>0xc0005013d0</t>
+  </si>
+  <si>
+    <t>0xc0005013e0</t>
+  </si>
+  <si>
+    <t>0xc0005013f0</t>
+  </si>
+  <si>
+    <t>0xc000506e58</t>
+  </si>
+  <si>
+    <t>0xc000506e68</t>
   </si>
   <si>
     <t>08-22-22</t>
   </si>
   <si>
-    <t>0xc00039e960</t>
-  </si>
-  <si>
-    <t>0xc00039e950</t>
-  </si>
-  <si>
-    <t>0xc00039e970</t>
-  </si>
-  <si>
-    <t>0xc00039e980</t>
-  </si>
-  <si>
-    <t>0xc00039e990</t>
-  </si>
-  <si>
-    <t>0xc0000252d0</t>
-  </si>
-  <si>
-    <t>0xc0000252e0</t>
+    <t>0xc000501410</t>
+  </si>
+  <si>
+    <t>0xc000501400</t>
+  </si>
+  <si>
+    <t>0xc000501420</t>
+  </si>
+  <si>
+    <t>0xc000501430</t>
+  </si>
+  <si>
+    <t>0xc000501440</t>
+  </si>
+  <si>
+    <t>0xc000506e90</t>
+  </si>
+  <si>
+    <t>0xc000506ea0</t>
   </si>
   <si>
     <t>09-22-02</t>
   </si>
   <si>
-    <t>0xc00039e9b0</t>
-  </si>
-  <si>
-    <t>0xc00039e9a0</t>
-  </si>
-  <si>
-    <t>0xc00039e9c0</t>
-  </si>
-  <si>
-    <t>0xc00039e9d0</t>
-  </si>
-  <si>
-    <t>0xc00039e9e0</t>
-  </si>
-  <si>
-    <t>0xc000025310</t>
-  </si>
-  <si>
-    <t>0xc000025320</t>
+    <t>0xc000501460</t>
+  </si>
+  <si>
+    <t>0xc000501450</t>
+  </si>
+  <si>
+    <t>0xc000501470</t>
+  </si>
+  <si>
+    <t>0xc000501480</t>
+  </si>
+  <si>
+    <t>0xc000501490</t>
+  </si>
+  <si>
+    <t>0xc000506ed0</t>
+  </si>
+  <si>
+    <t>0xc000506ee0</t>
   </si>
   <si>
     <t>10-22-01</t>
   </si>
   <si>
-    <t>0xc00039ea10</t>
-  </si>
-  <si>
-    <t>0xc00039ea00</t>
-  </si>
-  <si>
-    <t>0xc00039ea20</t>
-  </si>
-  <si>
-    <t>0xc00039ea30</t>
-  </si>
-  <si>
-    <t>0xc00039ea40</t>
-  </si>
-  <si>
-    <t>0xc000025340</t>
-  </si>
-  <si>
-    <t>0xc000025350</t>
+    <t>0xc0005014b0</t>
+  </si>
+  <si>
+    <t>0xc0005014a0</t>
+  </si>
+  <si>
+    <t>0xc0005014c0</t>
+  </si>
+  <si>
+    <t>0xc0005014d0</t>
+  </si>
+  <si>
+    <t>0xc0005014e0</t>
+  </si>
+  <si>
+    <t>0xc000506f00</t>
+  </si>
+  <si>
+    <t>0xc000506f10</t>
   </si>
   <si>
     <t>10-22-02</t>
   </si>
   <si>
-    <t>0xc00039ea80</t>
-  </si>
-  <si>
-    <t>0xc00039ea60</t>
-  </si>
-  <si>
-    <t>0xc00039eaa0</t>
-  </si>
-  <si>
-    <t>0xc00039eac0</t>
-  </si>
-  <si>
-    <t>0xc00039ead0</t>
-  </si>
-  <si>
-    <t>0xc000025370</t>
-  </si>
-  <si>
-    <t>0xc000025380</t>
+    <t>0xc000501500</t>
+  </si>
+  <si>
+    <t>0xc0005014f0</t>
+  </si>
+  <si>
+    <t>0xc000501510</t>
+  </si>
+  <si>
+    <t>0xc000501520</t>
+  </si>
+  <si>
+    <t>0xc000501530</t>
+  </si>
+  <si>
+    <t>0xc000506f30</t>
+  </si>
+  <si>
+    <t>0xc000506f40</t>
   </si>
   <si>
     <t>10-22-03</t>
   </si>
   <si>
-    <t>0xc00039eb00</t>
-  </si>
-  <si>
-    <t>0xc00039eaf0</t>
-  </si>
-  <si>
-    <t>0xc00039eb10</t>
-  </si>
-  <si>
-    <t>0xc00039eb20</t>
-  </si>
-  <si>
-    <t>0xc00039eb30</t>
-  </si>
-  <si>
-    <t>0xc0000253b8</t>
-  </si>
-  <si>
-    <t>0xc0000253f8</t>
+    <t>0xc000501550</t>
+  </si>
+  <si>
+    <t>0xc000501540</t>
+  </si>
+  <si>
+    <t>0xc000501560</t>
+  </si>
+  <si>
+    <t>0xc000501570</t>
+  </si>
+  <si>
+    <t>0xc000501580</t>
+  </si>
+  <si>
+    <t>0xc000506f58</t>
+  </si>
+  <si>
+    <t>0xc000506f78</t>
   </si>
   <si>
     <t>10-22-04</t>
   </si>
   <si>
-    <t>0xc00039eb50</t>
-  </si>
-  <si>
-    <t>0xc00039eb40</t>
-  </si>
-  <si>
-    <t>0xc00039eb60</t>
-  </si>
-  <si>
-    <t>0xc00039eb70</t>
-  </si>
-  <si>
-    <t>0xc00039eb80</t>
-  </si>
-  <si>
-    <t>0xc000025410</t>
-  </si>
-  <si>
-    <t>0xc000025420</t>
+    <t>0xc0005015a0</t>
+  </si>
+  <si>
+    <t>0xc000501590</t>
+  </si>
+  <si>
+    <t>0xc0005015b0</t>
+  </si>
+  <si>
+    <t>0xc0005015c0</t>
+  </si>
+  <si>
+    <t>0xc0005015d0</t>
+  </si>
+  <si>
+    <t>0xc000506f90</t>
+  </si>
+  <si>
+    <t>0xc000506fa0</t>
   </si>
   <si>
     <t>10-22-05</t>
   </si>
   <si>
-    <t>0xc00039eba0</t>
-  </si>
-  <si>
-    <t>0xc00039eb90</t>
-  </si>
-  <si>
-    <t>0xc00039ebb0</t>
-  </si>
-  <si>
-    <t>0xc00039ebc0</t>
-  </si>
-  <si>
-    <t>0xc00039ebd0</t>
-  </si>
-  <si>
-    <t>0xc000025440</t>
-  </si>
-  <si>
-    <t>0xc000025450</t>
+    <t>0xc0005015f0</t>
+  </si>
+  <si>
+    <t>0xc0005015e0</t>
+  </si>
+  <si>
+    <t>0xc000501600</t>
+  </si>
+  <si>
+    <t>0xc000501610</t>
+  </si>
+  <si>
+    <t>0xc000501620</t>
+  </si>
+  <si>
+    <t>0xc000506fc0</t>
+  </si>
+  <si>
+    <t>0xc000506fd0</t>
   </si>
   <si>
     <t>10-22-06</t>
   </si>
   <si>
-    <t>0xc00039ebf0</t>
-  </si>
-  <si>
-    <t>0xc00039ebe0</t>
-  </si>
-  <si>
-    <t>0xc00039ec00</t>
-  </si>
-  <si>
-    <t>0xc00039ec10</t>
-  </si>
-  <si>
-    <t>0xc00039ec20</t>
-  </si>
-  <si>
-    <t>0xc000025470</t>
-  </si>
-  <si>
-    <t>0xc000025480</t>
+    <t>0xc000501640</t>
+  </si>
+  <si>
+    <t>0xc000501630</t>
+  </si>
+  <si>
+    <t>0xc000501650</t>
+  </si>
+  <si>
+    <t>0xc000501660</t>
+  </si>
+  <si>
+    <t>0xc000501670</t>
+  </si>
+  <si>
+    <t>0xc000506ff0</t>
+  </si>
+  <si>
+    <t>0xc000507000</t>
   </si>
   <si>
     <t>10-22-07</t>
   </si>
   <si>
-    <t>0xc00039ec40</t>
-  </si>
-  <si>
-    <t>0xc00039ec30</t>
-  </si>
-  <si>
-    <t>0xc00039ec50</t>
-  </si>
-  <si>
-    <t>0xc00039ec60</t>
-  </si>
-  <si>
-    <t>0xc00039ec70</t>
-  </si>
-  <si>
-    <t>0xc0000254b0</t>
-  </si>
-  <si>
-    <t>0xc0000254d0</t>
+    <t>0xc000501690</t>
+  </si>
+  <si>
+    <t>0xc000501680</t>
+  </si>
+  <si>
+    <t>0xc0005016a0</t>
+  </si>
+  <si>
+    <t>0xc0005016b0</t>
+  </si>
+  <si>
+    <t>0xc0005016c0</t>
+  </si>
+  <si>
+    <t>0xc000507020</t>
+  </si>
+  <si>
+    <t>0xc000507030</t>
   </si>
   <si>
     <t>10-22-08</t>
   </si>
   <si>
-    <t>0xc00039eca0</t>
-  </si>
-  <si>
-    <t>0xc00039ec90</t>
-  </si>
-  <si>
-    <t>0xc00039ecb0</t>
-  </si>
-  <si>
-    <t>0xc00039ecd0</t>
-  </si>
-  <si>
-    <t>0xc00039ecf0</t>
-  </si>
-  <si>
-    <t>0xc000025500</t>
-  </si>
-  <si>
-    <t>0xc000025510</t>
+    <t>0xc0005016e0</t>
+  </si>
+  <si>
+    <t>0xc0005016d0</t>
+  </si>
+  <si>
+    <t>0xc0005016f0</t>
+  </si>
+  <si>
+    <t>0xc000501700</t>
+  </si>
+  <si>
+    <t>0xc000501710</t>
+  </si>
+  <si>
+    <t>0xc000507050</t>
+  </si>
+  <si>
+    <t>0xc000507060</t>
   </si>
   <si>
     <t>10-22-09</t>
   </si>
   <si>
-    <t>0xc00039ed10</t>
-  </si>
-  <si>
-    <t>0xc00039ed00</t>
-  </si>
-  <si>
-    <t>0xc00039ed20</t>
-  </si>
-  <si>
-    <t>0xc00039ed30</t>
-  </si>
-  <si>
-    <t>0xc00039ed40</t>
-  </si>
-  <si>
-    <t>0xc000025570</t>
-  </si>
-  <si>
-    <t>0xc0000255a0</t>
+    <t>0xc000501730</t>
+  </si>
+  <si>
+    <t>0xc000501720</t>
+  </si>
+  <si>
+    <t>0xc000501740</t>
+  </si>
+  <si>
+    <t>0xc000501750</t>
+  </si>
+  <si>
+    <t>0xc000501760</t>
+  </si>
+  <si>
+    <t>0xc000507080</t>
+  </si>
+  <si>
+    <t>0xc000507090</t>
   </si>
   <si>
     <t>10-22-10</t>
   </si>
   <si>
-    <t>0xc00039ed60</t>
-  </si>
-  <si>
-    <t>0xc00039ed50</t>
-  </si>
-  <si>
-    <t>0xc00039ed70</t>
-  </si>
-  <si>
-    <t>0xc00039ed80</t>
-  </si>
-  <si>
-    <t>0xc00039ed90</t>
-  </si>
-  <si>
-    <t>0xc0000255b8</t>
-  </si>
-  <si>
-    <t>0xc0000255e8</t>
+    <t>0xc000501780</t>
+  </si>
+  <si>
+    <t>0xc000501770</t>
+  </si>
+  <si>
+    <t>0xc000501790</t>
+  </si>
+  <si>
+    <t>0xc0005017a0</t>
+  </si>
+  <si>
+    <t>0xc0005017b0</t>
+  </si>
+  <si>
+    <t>0xc0005070a8</t>
+  </si>
+  <si>
+    <t>0xc0005070c8</t>
   </si>
   <si>
     <t>10-22-11</t>
   </si>
   <si>
-    <t>0xc00039edb0</t>
-  </si>
-  <si>
-    <t>0xc00039eda0</t>
-  </si>
-  <si>
-    <t>0xc00039edc0</t>
-  </si>
-  <si>
-    <t>0xc00039edd0</t>
-  </si>
-  <si>
-    <t>0xc00039ede0</t>
-  </si>
-  <si>
-    <t>0xc000025630</t>
-  </si>
-  <si>
-    <t>0xc000025640</t>
+    <t>0xc0005017d0</t>
+  </si>
+  <si>
+    <t>0xc0005017c0</t>
+  </si>
+  <si>
+    <t>0xc0005017e0</t>
+  </si>
+  <si>
+    <t>0xc0005017f0</t>
+  </si>
+  <si>
+    <t>0xc000501800</t>
+  </si>
+  <si>
+    <t>0xc0005070f0</t>
+  </si>
+  <si>
+    <t>0xc000507100</t>
   </si>
   <si>
     <t>10-22-12</t>
   </si>
   <si>
-    <t>0xc00039ee00</t>
-  </si>
-  <si>
-    <t>0xc00039edf0</t>
-  </si>
-  <si>
-    <t>0xc00039ee10</t>
-  </si>
-  <si>
-    <t>0xc00039ee20</t>
-  </si>
-  <si>
-    <t>0xc00039ee30</t>
-  </si>
-  <si>
-    <t>0xc000025670</t>
-  </si>
-  <si>
-    <t>0xc000025690</t>
+    <t>0xc000501820</t>
+  </si>
+  <si>
+    <t>0xc000501810</t>
+  </si>
+  <si>
+    <t>0xc000501830</t>
+  </si>
+  <si>
+    <t>0xc000501840</t>
+  </si>
+  <si>
+    <t>0xc000501850</t>
+  </si>
+  <si>
+    <t>0xc000507120</t>
+  </si>
+  <si>
+    <t>0xc000507150</t>
   </si>
   <si>
     <t>10-22-13</t>
   </si>
   <si>
-    <t>0xc00039ee50</t>
-  </si>
-  <si>
-    <t>0xc00039ee40</t>
-  </si>
-  <si>
-    <t>0xc00039ee60</t>
-  </si>
-  <si>
-    <t>0xc00039ee70</t>
-  </si>
-  <si>
-    <t>0xc00039ee80</t>
-  </si>
-  <si>
-    <t>0xc0000256a8</t>
-  </si>
-  <si>
-    <t>0xc0000256b8</t>
+    <t>0xc000501870</t>
+  </si>
+  <si>
+    <t>0xc000501860</t>
+  </si>
+  <si>
+    <t>0xc000501880</t>
+  </si>
+  <si>
+    <t>0xc000501890</t>
+  </si>
+  <si>
+    <t>0xc0005018a0</t>
+  </si>
+  <si>
+    <t>0xc000507188</t>
+  </si>
+  <si>
+    <t>0xc000507198</t>
   </si>
   <si>
     <t>10-22-14</t>
   </si>
   <si>
-    <t>0xc00039eea0</t>
-  </si>
-  <si>
-    <t>0xc00039ee90</t>
-  </si>
-  <si>
-    <t>0xc00039eec0</t>
-  </si>
-  <si>
-    <t>0xc00039eee0</t>
-  </si>
-  <si>
-    <t>0xc00039eef0</t>
-  </si>
-  <si>
-    <t>0xc0000256e0</t>
-  </si>
-  <si>
-    <t>0xc0000256f0</t>
+    <t>0xc0005018c0</t>
+  </si>
+  <si>
+    <t>0xc0005018b0</t>
+  </si>
+  <si>
+    <t>0xc0005018d0</t>
+  </si>
+  <si>
+    <t>0xc0005018e0</t>
+  </si>
+  <si>
+    <t>0xc0005018f0</t>
+  </si>
+  <si>
+    <t>0xc0005071c0</t>
+  </si>
+  <si>
+    <t>0xc0005071d0</t>
   </si>
   <si>
     <t>10-22-15</t>
   </si>
   <si>
-    <t>0xc00039ef10</t>
-  </si>
-  <si>
-    <t>0xc00039ef00</t>
-  </si>
-  <si>
-    <t>0xc00039ef20</t>
-  </si>
-  <si>
-    <t>0xc00039ef40</t>
-  </si>
-  <si>
-    <t>0xc00039ef60</t>
-  </si>
-  <si>
-    <t>0xc000025710</t>
-  </si>
-  <si>
-    <t>0xc000025720</t>
+    <t>0xc000501910</t>
+  </si>
+  <si>
+    <t>0xc000501900</t>
+  </si>
+  <si>
+    <t>0xc000501920</t>
+  </si>
+  <si>
+    <t>0xc000501930</t>
+  </si>
+  <si>
+    <t>0xc000501940</t>
+  </si>
+  <si>
+    <t>0xc0005071f0</t>
+  </si>
+  <si>
+    <t>0xc000507200</t>
   </si>
   <si>
     <t>10-22-16</t>
   </si>
   <si>
-    <t>0xc00039ef90</t>
-  </si>
-  <si>
-    <t>0xc00039ef70</t>
-  </si>
-  <si>
-    <t>0xc00039efa0</t>
-  </si>
-  <si>
-    <t>0xc00039efb0</t>
-  </si>
-  <si>
-    <t>0xc00039efe0</t>
-  </si>
-  <si>
-    <t>0xc000025740</t>
-  </si>
-  <si>
-    <t>0xc000025750</t>
+    <t>0xc000501960</t>
+  </si>
+  <si>
+    <t>0xc000501950</t>
+  </si>
+  <si>
+    <t>0xc000501970</t>
+  </si>
+  <si>
+    <t>0xc000501980</t>
+  </si>
+  <si>
+    <t>0xc000501990</t>
+  </si>
+  <si>
+    <t>0xc000507220</t>
+  </si>
+  <si>
+    <t>0xc000507230</t>
   </si>
   <si>
     <t>10-22-17</t>
   </si>
   <si>
-    <t>0xc00039f000</t>
-  </si>
-  <si>
-    <t>0xc00039eff0</t>
-  </si>
-  <si>
-    <t>0xc00039f010</t>
-  </si>
-  <si>
-    <t>0xc00039f020</t>
-  </si>
-  <si>
-    <t>0xc00039f040</t>
-  </si>
-  <si>
-    <t>0xc000025770</t>
-  </si>
-  <si>
-    <t>0xc000025780</t>
+    <t>0xc0005019b0</t>
+  </si>
+  <si>
+    <t>0xc0005019a0</t>
+  </si>
+  <si>
+    <t>0xc0005019c0</t>
+  </si>
+  <si>
+    <t>0xc0005019d0</t>
+  </si>
+  <si>
+    <t>0xc0005019e0</t>
+  </si>
+  <si>
+    <t>0xc000507250</t>
+  </si>
+  <si>
+    <t>0xc000507260</t>
   </si>
   <si>
     <t>10-22-18</t>
   </si>
   <si>
-    <t>0xc00039f060</t>
-  </si>
-  <si>
-    <t>0xc00039f050</t>
-  </si>
-  <si>
-    <t>0xc00039f070</t>
-  </si>
-  <si>
-    <t>0xc00039f080</t>
-  </si>
-  <si>
-    <t>0xc00039f0a0</t>
-  </si>
-  <si>
-    <t>0xc000025798</t>
-  </si>
-  <si>
-    <t>0xc0000257a8</t>
+    <t>0xc000501a00</t>
+  </si>
+  <si>
+    <t>0xc0005019f0</t>
+  </si>
+  <si>
+    <t>0xc000501a10</t>
+  </si>
+  <si>
+    <t>0xc000501a20</t>
+  </si>
+  <si>
+    <t>0xc000501a30</t>
+  </si>
+  <si>
+    <t>0xc000507278</t>
+  </si>
+  <si>
+    <t>0xc000507288</t>
   </si>
   <si>
     <t>123456</t>
@@ -1954,484 +1954,484 @@
     <t>&lt;nil&gt;</t>
   </si>
   <si>
-    <t>0xc00039f0b0</t>
-  </si>
-  <si>
-    <t>0xc00039f0c0</t>
-  </si>
-  <si>
-    <t>0xc00039f0d0</t>
-  </si>
-  <si>
-    <t>0xc00039f0e0</t>
-  </si>
-  <si>
-    <t>0xc0000257b8</t>
-  </si>
-  <si>
-    <t>0xc0000257c8</t>
+    <t>0xc000501a40</t>
+  </si>
+  <si>
+    <t>0xc000501a50</t>
+  </si>
+  <si>
+    <t>0xc000501a60</t>
+  </si>
+  <si>
+    <t>0xc000501a70</t>
+  </si>
+  <si>
+    <t>0xc000507298</t>
+  </si>
+  <si>
+    <t>0xc0005072a8</t>
   </si>
   <si>
     <t>CAP-112</t>
   </si>
   <si>
-    <t>0xc00039f100</t>
+    <t>0xc000501a90</t>
   </si>
   <si>
     <t>H</t>
   </si>
   <si>
-    <t>0xc00039f0f0</t>
-  </si>
-  <si>
-    <t>0xc00039f110</t>
-  </si>
-  <si>
-    <t>0xc00039f130</t>
-  </si>
-  <si>
-    <t>0xc00039f150</t>
-  </si>
-  <si>
-    <t>0xc0000257d8</t>
-  </si>
-  <si>
-    <t>0xc0000257e8</t>
+    <t>0xc000501a80</t>
+  </si>
+  <si>
+    <t>0xc000501aa0</t>
+  </si>
+  <si>
+    <t>0xc000501ab0</t>
+  </si>
+  <si>
+    <t>0xc000501ac0</t>
+  </si>
+  <si>
+    <t>0xc0005072b8</t>
+  </si>
+  <si>
+    <t>0xc0005072c8</t>
   </si>
   <si>
     <t>CAP-144</t>
   </si>
   <si>
-    <t>0xc00039f170</t>
+    <t>0xc000501ae0</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>0xc00039f160</t>
-  </si>
-  <si>
-    <t>0xc00039f180</t>
-  </si>
-  <si>
-    <t>0xc00039f190</t>
-  </si>
-  <si>
-    <t>0xc00039f1a0</t>
-  </si>
-  <si>
-    <t>0xc0000257f8</t>
-  </si>
-  <si>
-    <t>0xc000025818</t>
+    <t>0xc000501ad0</t>
+  </si>
+  <si>
+    <t>0xc000501af0</t>
+  </si>
+  <si>
+    <t>0xc000501b00</t>
+  </si>
+  <si>
+    <t>0xc000501b10</t>
+  </si>
+  <si>
+    <t>0xc0005072d8</t>
+  </si>
+  <si>
+    <t>0xc0005072f8</t>
   </si>
   <si>
     <t>CAP-198</t>
   </si>
   <si>
-    <t>0xc00039f1c0</t>
-  </si>
-  <si>
-    <t>0xc00039f1b0</t>
-  </si>
-  <si>
-    <t>0xc00039f1e0</t>
-  </si>
-  <si>
-    <t>0xc00039f1f0</t>
-  </si>
-  <si>
-    <t>0xc00039f200</t>
-  </si>
-  <si>
-    <t>0xc000025828</t>
-  </si>
-  <si>
-    <t>0xc000025848</t>
+    <t>0xc000501b30</t>
+  </si>
+  <si>
+    <t>0xc000501b20</t>
+  </si>
+  <si>
+    <t>0xc000501b40</t>
+  </si>
+  <si>
+    <t>0xc000501b50</t>
+  </si>
+  <si>
+    <t>0xc000501b60</t>
+  </si>
+  <si>
+    <t>0xc000507308</t>
+  </si>
+  <si>
+    <t>0xc000507328</t>
   </si>
   <si>
     <t>CAP-205</t>
   </si>
   <si>
-    <t>0xc00039f230</t>
-  </si>
-  <si>
-    <t>0xc00039f220</t>
-  </si>
-  <si>
-    <t>0xc00039f260</t>
-  </si>
-  <si>
-    <t>0xc00039f270</t>
-  </si>
-  <si>
-    <t>0xc00039f280</t>
-  </si>
-  <si>
-    <t>0xc000025858</t>
-  </si>
-  <si>
-    <t>0xc000025878</t>
+    <t>0xc000501b80</t>
+  </si>
+  <si>
+    <t>0xc000501b70</t>
+  </si>
+  <si>
+    <t>0xc000501b90</t>
+  </si>
+  <si>
+    <t>0xc000501ba0</t>
+  </si>
+  <si>
+    <t>0xc000501bb0</t>
+  </si>
+  <si>
+    <t>0xc000507338</t>
+  </si>
+  <si>
+    <t>0xc000507358</t>
   </si>
   <si>
     <t>CAP-225</t>
   </si>
   <si>
-    <t>0xc00039f2a0</t>
-  </si>
-  <si>
-    <t>0xc00039f290</t>
-  </si>
-  <si>
-    <t>0xc00039f2b0</t>
-  </si>
-  <si>
-    <t>0xc00039f2c0</t>
-  </si>
-  <si>
-    <t>0xc00039f2d0</t>
-  </si>
-  <si>
-    <t>0xc000025888</t>
-  </si>
-  <si>
-    <t>0xc000025898</t>
+    <t>0xc000501bd0</t>
+  </si>
+  <si>
+    <t>0xc000501bc0</t>
+  </si>
+  <si>
+    <t>0xc000501be0</t>
+  </si>
+  <si>
+    <t>0xc000501bf0</t>
+  </si>
+  <si>
+    <t>0xc000501c00</t>
+  </si>
+  <si>
+    <t>0xc000507368</t>
+  </si>
+  <si>
+    <t>0xc000507378</t>
   </si>
   <si>
     <t>CAP-230</t>
   </si>
   <si>
-    <t>0xc00039f2f0</t>
-  </si>
-  <si>
-    <t>0xc00039f2e0</t>
-  </si>
-  <si>
-    <t>0xc00039f300</t>
-  </si>
-  <si>
-    <t>0xc00039f310</t>
-  </si>
-  <si>
-    <t>0xc00039f320</t>
-  </si>
-  <si>
-    <t>0xc0000258a8</t>
-  </si>
-  <si>
-    <t>0xc0000258d8</t>
+    <t>0xc000501c20</t>
+  </si>
+  <si>
+    <t>0xc000501c10</t>
+  </si>
+  <si>
+    <t>0xc000501c30</t>
+  </si>
+  <si>
+    <t>0xc000501c40</t>
+  </si>
+  <si>
+    <t>0xc000501c50</t>
+  </si>
+  <si>
+    <t>0xc000507388</t>
+  </si>
+  <si>
+    <t>0xc0005073a8</t>
   </si>
   <si>
     <t>CAP-251</t>
   </si>
   <si>
-    <t>0xc00039f340</t>
-  </si>
-  <si>
-    <t>0xc00039f330</t>
-  </si>
-  <si>
-    <t>0xc00039f350</t>
-  </si>
-  <si>
-    <t>0xc00039f360</t>
-  </si>
-  <si>
-    <t>0xc00039f380</t>
-  </si>
-  <si>
-    <t>0xc0000258f8</t>
-  </si>
-  <si>
-    <t>0xc000025928</t>
+    <t>0xc000501c70</t>
+  </si>
+  <si>
+    <t>0xc000501c60</t>
+  </si>
+  <si>
+    <t>0xc000501c80</t>
+  </si>
+  <si>
+    <t>0xc000501c90</t>
+  </si>
+  <si>
+    <t>0xc000501ca0</t>
+  </si>
+  <si>
+    <t>0xc0005073b8</t>
+  </si>
+  <si>
+    <t>0xc0005073d8</t>
   </si>
   <si>
     <t>CAP-260</t>
   </si>
   <si>
-    <t>0xc00039f3b0</t>
-  </si>
-  <si>
-    <t>0xc00039f390</t>
-  </si>
-  <si>
-    <t>0xc00039f3c0</t>
-  </si>
-  <si>
-    <t>0xc00039f3d0</t>
-  </si>
-  <si>
-    <t>0xc00039f3e0</t>
-  </si>
-  <si>
-    <t>0xc000025938</t>
-  </si>
-  <si>
-    <t>0xc000025998</t>
+    <t>0xc000501cc0</t>
+  </si>
+  <si>
+    <t>0xc000501cb0</t>
+  </si>
+  <si>
+    <t>0xc000501cd0</t>
+  </si>
+  <si>
+    <t>0xc000501ce0</t>
+  </si>
+  <si>
+    <t>0xc000501cf0</t>
+  </si>
+  <si>
+    <t>0xc0005073e8</t>
+  </si>
+  <si>
+    <t>0xc000507408</t>
   </si>
   <si>
     <t>CAP-263</t>
   </si>
   <si>
-    <t>0xc00039f410</t>
-  </si>
-  <si>
-    <t>0xc00039f400</t>
-  </si>
-  <si>
-    <t>0xc00039f430</t>
-  </si>
-  <si>
-    <t>0xc00039f440</t>
-  </si>
-  <si>
-    <t>0xc00039f450</t>
-  </si>
-  <si>
-    <t>0xc0000259f0</t>
-  </si>
-  <si>
-    <t>0xc000025a00</t>
+    <t>0xc000501d10</t>
+  </si>
+  <si>
+    <t>0xc000501d00</t>
+  </si>
+  <si>
+    <t>0xc000501d20</t>
+  </si>
+  <si>
+    <t>0xc000501d30</t>
+  </si>
+  <si>
+    <t>0xc000501d40</t>
+  </si>
+  <si>
+    <t>0xc000507430</t>
+  </si>
+  <si>
+    <t>0xc000507440</t>
   </si>
   <si>
     <t>CAP-272</t>
   </si>
   <si>
-    <t>0xc00039f470</t>
-  </si>
-  <si>
-    <t>0xc00039f460</t>
-  </si>
-  <si>
-    <t>0xc00039f480</t>
-  </si>
-  <si>
-    <t>0xc00039f490</t>
-  </si>
-  <si>
-    <t>0xc00039f4b0</t>
-  </si>
-  <si>
-    <t>0xc000025a30</t>
-  </si>
-  <si>
-    <t>0xc000025a50</t>
+    <t>0xc000501d60</t>
+  </si>
+  <si>
+    <t>0xc000501d50</t>
+  </si>
+  <si>
+    <t>0xc000501d70</t>
+  </si>
+  <si>
+    <t>0xc000501d80</t>
+  </si>
+  <si>
+    <t>0xc000501d90</t>
+  </si>
+  <si>
+    <t>0xc000507460</t>
+  </si>
+  <si>
+    <t>0xc000507470</t>
   </si>
   <si>
     <t>CAP-312</t>
   </si>
   <si>
-    <t>0xc00039f4d0</t>
-  </si>
-  <si>
-    <t>0xc00039f4c0</t>
-  </si>
-  <si>
-    <t>0xc00039f4f0</t>
-  </si>
-  <si>
-    <t>0xc00039f500</t>
-  </si>
-  <si>
-    <t>0xc00039f510</t>
-  </si>
-  <si>
-    <t>0xc000025a88</t>
-  </si>
-  <si>
-    <t>0xc000025ab0</t>
+    <t>0xc000501db0</t>
+  </si>
+  <si>
+    <t>0xc000501da0</t>
+  </si>
+  <si>
+    <t>0xc000501dc0</t>
+  </si>
+  <si>
+    <t>0xc000501dd0</t>
+  </si>
+  <si>
+    <t>0xc000501de0</t>
+  </si>
+  <si>
+    <t>0xc000507498</t>
+  </si>
+  <si>
+    <t>0xc0005074b0</t>
   </si>
   <si>
     <t>CAP-313</t>
   </si>
   <si>
-    <t>0xc00039f530</t>
-  </si>
-  <si>
-    <t>0xc00039f520</t>
-  </si>
-  <si>
-    <t>0xc00039f550</t>
-  </si>
-  <si>
-    <t>0xc00039f560</t>
-  </si>
-  <si>
-    <t>0xc00039f570</t>
-  </si>
-  <si>
-    <t>0xc000025ac8</t>
-  </si>
-  <si>
-    <t>0xc000025af0</t>
+    <t>0xc000501e00</t>
+  </si>
+  <si>
+    <t>0xc000501df0</t>
+  </si>
+  <si>
+    <t>0xc000501e10</t>
+  </si>
+  <si>
+    <t>0xc000501e20</t>
+  </si>
+  <si>
+    <t>0xc000501e30</t>
+  </si>
+  <si>
+    <t>0xc0005074c8</t>
+  </si>
+  <si>
+    <t>0xc0005074e0</t>
   </si>
   <si>
     <t>CAP-314</t>
   </si>
   <si>
-    <t>0xc00039f5c0</t>
-  </si>
-  <si>
-    <t>0xc00039f5a0</t>
-  </si>
-  <si>
-    <t>0xc00039f5d0</t>
-  </si>
-  <si>
-    <t>0xc00039f5e0</t>
-  </si>
-  <si>
-    <t>0xc00039f5f0</t>
-  </si>
-  <si>
-    <t>0xc000025b18</t>
-  </si>
-  <si>
-    <t>0xc000025b40</t>
+    <t>0xc000501e50</t>
+  </si>
+  <si>
+    <t>0xc000501e40</t>
+  </si>
+  <si>
+    <t>0xc000501e60</t>
+  </si>
+  <si>
+    <t>0xc000501e70</t>
+  </si>
+  <si>
+    <t>0xc000501e80</t>
+  </si>
+  <si>
+    <t>0xc0005074f8</t>
+  </si>
+  <si>
+    <t>0xc000507510</t>
   </si>
   <si>
     <t>CAP-316</t>
   </si>
   <si>
-    <t>0xc00039f610</t>
-  </si>
-  <si>
-    <t>0xc00039f600</t>
-  </si>
-  <si>
-    <t>0xc00039f620</t>
-  </si>
-  <si>
-    <t>0xc00039f630</t>
-  </si>
-  <si>
-    <t>0xc00039f640</t>
-  </si>
-  <si>
-    <t>0xc000025b58</t>
-  </si>
-  <si>
-    <t>0xc000025bb0</t>
+    <t>0xc000501ea0</t>
+  </si>
+  <si>
+    <t>0xc000501e90</t>
+  </si>
+  <si>
+    <t>0xc000501eb0</t>
+  </si>
+  <si>
+    <t>0xc000501ec0</t>
+  </si>
+  <si>
+    <t>0xc000501ed0</t>
+  </si>
+  <si>
+    <t>0xc000507528</t>
+  </si>
+  <si>
+    <t>0xc000507540</t>
   </si>
   <si>
     <t>CAP-317</t>
   </si>
   <si>
-    <t>0xc00039f660</t>
-  </si>
-  <si>
-    <t>0xc00039f650</t>
-  </si>
-  <si>
-    <t>0xc00039f670</t>
-  </si>
-  <si>
-    <t>0xc00039f680</t>
-  </si>
-  <si>
-    <t>0xc00039f690</t>
-  </si>
-  <si>
-    <t>0xc000025be8</t>
-  </si>
-  <si>
-    <t>0xc000025c10</t>
+    <t>0xc000501ef0</t>
+  </si>
+  <si>
+    <t>0xc000501ee0</t>
+  </si>
+  <si>
+    <t>0xc000501f00</t>
+  </si>
+  <si>
+    <t>0xc000501f10</t>
+  </si>
+  <si>
+    <t>0xc000501f20</t>
+  </si>
+  <si>
+    <t>0xc000507558</t>
+  </si>
+  <si>
+    <t>0xc000507570</t>
   </si>
   <si>
     <t>CAP-320</t>
   </si>
   <si>
-    <t>0xc00039f6b0</t>
-  </si>
-  <si>
-    <t>0xc00039f6a0</t>
-  </si>
-  <si>
-    <t>0xc00039f6c0</t>
-  </si>
-  <si>
-    <t>0xc00039f6d0</t>
-  </si>
-  <si>
-    <t>0xc00039f6e0</t>
-  </si>
-  <si>
-    <t>0xc000025c40</t>
-  </si>
-  <si>
-    <t>0xc000025c50</t>
+    <t>0xc000501f40</t>
+  </si>
+  <si>
+    <t>0xc000501f30</t>
+  </si>
+  <si>
+    <t>0xc000501f50</t>
+  </si>
+  <si>
+    <t>0xc000501f60</t>
+  </si>
+  <si>
+    <t>0xc000501f70</t>
+  </si>
+  <si>
+    <t>0xc000507590</t>
+  </si>
+  <si>
+    <t>0xc0005075a0</t>
   </si>
   <si>
     <t>CAP-321</t>
   </si>
   <si>
-    <t>0xc00039f700</t>
-  </si>
-  <si>
-    <t>0xc00039f6f0</t>
-  </si>
-  <si>
-    <t>0xc00039f710</t>
-  </si>
-  <si>
-    <t>0xc00039f720</t>
-  </si>
-  <si>
-    <t>0xc00039f730</t>
-  </si>
-  <si>
-    <t>0xc000025c80</t>
-  </si>
-  <si>
-    <t>0xc000025ca0</t>
+    <t>0xc000501f90</t>
+  </si>
+  <si>
+    <t>0xc000501f80</t>
+  </si>
+  <si>
+    <t>0xc000501fa0</t>
+  </si>
+  <si>
+    <t>0xc000501fb0</t>
+  </si>
+  <si>
+    <t>0xc000501fc0</t>
+  </si>
+  <si>
+    <t>0xc0005075c0</t>
+  </si>
+  <si>
+    <t>0xc0005075d0</t>
   </si>
   <si>
     <t>CAP-322</t>
   </si>
   <si>
-    <t>0xc00039f750</t>
-  </si>
-  <si>
-    <t>0xc00039f740</t>
-  </si>
-  <si>
-    <t>0xc00039f760</t>
-  </si>
-  <si>
-    <t>0xc00039f770</t>
-  </si>
-  <si>
-    <t>0xc00039f780</t>
-  </si>
-  <si>
-    <t>0xc000025cd8</t>
-  </si>
-  <si>
-    <t>0xc000025ce8</t>
+    <t>0xc000501fe0</t>
+  </si>
+  <si>
+    <t>0xc000501fd0</t>
+  </si>
+  <si>
+    <t>0xc000501ff0</t>
+  </si>
+  <si>
+    <t>0xc00009c000</t>
+  </si>
+  <si>
+    <t>0xc00009c010</t>
+  </si>
+  <si>
+    <t>0xc0005075f8</t>
+  </si>
+  <si>
+    <t>0xc000507608</t>
   </si>
   <si>
     <t>CAP-323</t>
   </si>
   <si>
-    <t>0xc00039f7a0</t>
-  </si>
-  <si>
-    <t>0xc00039f790</t>
-  </si>
-  <si>
-    <t>0xc00039f7b0</t>
-  </si>
-  <si>
-    <t>0xc00039f7c0</t>
-  </si>
-  <si>
-    <t>0xc00039f7d0</t>
-  </si>
-  <si>
-    <t>0xc000025d10</t>
-  </si>
-  <si>
-    <t>0xc000025d28</t>
+    <t>0xc00009c030</t>
+  </si>
+  <si>
+    <t>0xc00009c020</t>
+  </si>
+  <si>
+    <t>0xc00009c040</t>
+  </si>
+  <si>
+    <t>0xc00009c050</t>
+  </si>
+  <si>
+    <t>0xc00009c060</t>
+  </si>
+  <si>
+    <t>0xc000507630</t>
+  </si>
+  <si>
+    <t>0xc000507648</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
added 'modified' field to the product
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -19,1933 +19,1933 @@
     <t>"09-22-01</t>
   </si>
   <si>
-    <t>0xc0005000c0</t>
+    <t>0xc0000ba5a0</t>
   </si>
   <si>
     <t>PW</t>
   </si>
   <si>
-    <t>0xc0005000b0</t>
-  </si>
-  <si>
-    <t>0xc0005000d0</t>
-  </si>
-  <si>
-    <t>0xc0005000e0</t>
-  </si>
-  <si>
-    <t>0xc0005000f0</t>
-  </si>
-  <si>
-    <t>0xc0005060e8</t>
+    <t>0xc0000ba590</t>
+  </si>
+  <si>
+    <t>0xc0000ba5b0</t>
+  </si>
+  <si>
+    <t>0xc0000ba5c0</t>
+  </si>
+  <si>
+    <t>0xc0000ba5d0</t>
+  </si>
+  <si>
+    <t>0xc00042e2d8</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
-    <t>0xc0005060f8</t>
+    <t>0xc00042e2f8</t>
   </si>
   <si>
     <t>"09-22-03</t>
   </si>
   <si>
-    <t>0xc000500110</t>
-  </si>
-  <si>
-    <t>0xc000500100</t>
-  </si>
-  <si>
-    <t>0xc000500120</t>
-  </si>
-  <si>
-    <t>0xc000500130</t>
-  </si>
-  <si>
-    <t>0xc000500140</t>
-  </si>
-  <si>
-    <t>0xc000506130</t>
-  </si>
-  <si>
-    <t>0xc000506140</t>
+    <t>0xc0000ba600</t>
+  </si>
+  <si>
+    <t>0xc0000ba5f0</t>
+  </si>
+  <si>
+    <t>0xc0000ba610</t>
+  </si>
+  <si>
+    <t>0xc0000ba620</t>
+  </si>
+  <si>
+    <t>0xc0000ba630</t>
+  </si>
+  <si>
+    <t>0xc00042e340</t>
+  </si>
+  <si>
+    <t>0xc00042e350</t>
   </si>
   <si>
     <t>"09-22-04</t>
   </si>
   <si>
-    <t>0xc000500160</t>
-  </si>
-  <si>
-    <t>0xc000500150</t>
-  </si>
-  <si>
-    <t>0xc000500170</t>
-  </si>
-  <si>
-    <t>0xc000500180</t>
-  </si>
-  <si>
-    <t>0xc000500190</t>
-  </si>
-  <si>
-    <t>0xc000506178</t>
-  </si>
-  <si>
-    <t>0xc000506188</t>
+    <t>0xc0000ba660</t>
+  </si>
+  <si>
+    <t>0xc0000ba650</t>
+  </si>
+  <si>
+    <t>0xc0000ba670</t>
+  </si>
+  <si>
+    <t>0xc0000ba680</t>
+  </si>
+  <si>
+    <t>0xc0000ba690</t>
+  </si>
+  <si>
+    <t>0xc00042e3b8</t>
+  </si>
+  <si>
+    <t>0xc00042e3c8</t>
   </si>
   <si>
     <t>"09-22-05</t>
   </si>
   <si>
-    <t>0xc0005001b0</t>
-  </si>
-  <si>
-    <t>0xc0005001a0</t>
-  </si>
-  <si>
-    <t>0xc0005001c0</t>
-  </si>
-  <si>
-    <t>0xc0005001d0</t>
-  </si>
-  <si>
-    <t>0xc0005001e0</t>
-  </si>
-  <si>
-    <t>0xc0005061b8</t>
-  </si>
-  <si>
-    <t>0xc0005061c8</t>
+    <t>0xc0000ba6c0</t>
+  </si>
+  <si>
+    <t>0xc0000ba6b0</t>
+  </si>
+  <si>
+    <t>0xc0000ba6d0</t>
+  </si>
+  <si>
+    <t>0xc0000ba6e0</t>
+  </si>
+  <si>
+    <t>0xc0000ba6f0</t>
+  </si>
+  <si>
+    <t>0xc00042e3f8</t>
+  </si>
+  <si>
+    <t>0xc00042e408</t>
   </si>
   <si>
     <t>"09-22-06</t>
   </si>
   <si>
-    <t>0xc000500200</t>
-  </si>
-  <si>
-    <t>0xc0005001f0</t>
-  </si>
-  <si>
-    <t>0xc000500210</t>
-  </si>
-  <si>
-    <t>0xc000500220</t>
-  </si>
-  <si>
-    <t>0xc000500230</t>
-  </si>
-  <si>
-    <t>0xc000506200</t>
-  </si>
-  <si>
-    <t>0xc000506210</t>
+    <t>0xc0000ba730</t>
+  </si>
+  <si>
+    <t>0xc0000ba710</t>
+  </si>
+  <si>
+    <t>0xc0000ba740</t>
+  </si>
+  <si>
+    <t>0xc0000ba750</t>
+  </si>
+  <si>
+    <t>0xc0000ba760</t>
+  </si>
+  <si>
+    <t>0xc00042e440</t>
+  </si>
+  <si>
+    <t>0xc00042e450</t>
   </si>
   <si>
     <t>"09-22-07</t>
   </si>
   <si>
-    <t>0xc000500250</t>
-  </si>
-  <si>
-    <t>0xc000500240</t>
-  </si>
-  <si>
-    <t>0xc000500260</t>
-  </si>
-  <si>
-    <t>0xc000500270</t>
-  </si>
-  <si>
-    <t>0xc000500280</t>
-  </si>
-  <si>
-    <t>0xc000506240</t>
-  </si>
-  <si>
-    <t>0xc000506258</t>
+    <t>0xc0000ba7b0</t>
+  </si>
+  <si>
+    <t>0xc0000ba790</t>
+  </si>
+  <si>
+    <t>0xc0000ba7d0</t>
+  </si>
+  <si>
+    <t>0xc0000ba7f0</t>
+  </si>
+  <si>
+    <t>0xc0000ba800</t>
+  </si>
+  <si>
+    <t>0xc00042e480</t>
+  </si>
+  <si>
+    <t>0xc00042e498</t>
   </si>
   <si>
     <t>"09-22-08</t>
   </si>
   <si>
-    <t>0xc0005002a0</t>
-  </si>
-  <si>
-    <t>0xc000500290</t>
-  </si>
-  <si>
-    <t>0xc0005002b0</t>
-  </si>
-  <si>
-    <t>0xc0005002c0</t>
-  </si>
-  <si>
-    <t>0xc0005002d0</t>
-  </si>
-  <si>
-    <t>0xc000506280</t>
-  </si>
-  <si>
-    <t>0xc000506298</t>
+    <t>0xc0000ba840</t>
+  </si>
+  <si>
+    <t>0xc0000ba830</t>
+  </si>
+  <si>
+    <t>0xc0000ba850</t>
+  </si>
+  <si>
+    <t>0xc0000ba860</t>
+  </si>
+  <si>
+    <t>0xc0000ba870</t>
+  </si>
+  <si>
+    <t>0xc00042e4c0</t>
+  </si>
+  <si>
+    <t>0xc00042e4d8</t>
   </si>
   <si>
     <t>"09-22-09</t>
   </si>
   <si>
-    <t>0xc0005002f0</t>
-  </si>
-  <si>
-    <t>0xc0005002e0</t>
-  </si>
-  <si>
-    <t>0xc000500300</t>
-  </si>
-  <si>
-    <t>0xc000500310</t>
-  </si>
-  <si>
-    <t>0xc000500320</t>
-  </si>
-  <si>
-    <t>0xc0005062d8</t>
-  </si>
-  <si>
-    <t>0xc0005062f0</t>
+    <t>0xc0000ba8a0</t>
+  </si>
+  <si>
+    <t>0xc0000ba890</t>
+  </si>
+  <si>
+    <t>0xc0000ba8b0</t>
+  </si>
+  <si>
+    <t>0xc0000ba8c0</t>
+  </si>
+  <si>
+    <t>0xc0000ba8d0</t>
+  </si>
+  <si>
+    <t>0xc00042e518</t>
+  </si>
+  <si>
+    <t>0xc00042e530</t>
   </si>
   <si>
     <t>"09-22-10</t>
   </si>
   <si>
-    <t>0xc000500340</t>
-  </si>
-  <si>
-    <t>0xc000500330</t>
-  </si>
-  <si>
-    <t>0xc000500350</t>
-  </si>
-  <si>
-    <t>0xc000500360</t>
-  </si>
-  <si>
-    <t>0xc000500370</t>
-  </si>
-  <si>
-    <t>0xc000506330</t>
-  </si>
-  <si>
-    <t>0xc000506348</t>
+    <t>0xc0000ba900</t>
+  </si>
+  <si>
+    <t>0xc0000ba8f0</t>
+  </si>
+  <si>
+    <t>0xc0000ba910</t>
+  </si>
+  <si>
+    <t>0xc0000ba920</t>
+  </si>
+  <si>
+    <t>0xc0000ba930</t>
+  </si>
+  <si>
+    <t>0xc00042e570</t>
+  </si>
+  <si>
+    <t>0xc00042e588</t>
   </si>
   <si>
     <t>"09-22-11</t>
   </si>
   <si>
-    <t>0xc000500390</t>
-  </si>
-  <si>
-    <t>0xc000500380</t>
-  </si>
-  <si>
-    <t>0xc0005003a0</t>
-  </si>
-  <si>
-    <t>0xc0005003b0</t>
-  </si>
-  <si>
-    <t>0xc0005003c0</t>
-  </si>
-  <si>
-    <t>0xc000506380</t>
-  </si>
-  <si>
-    <t>0xc000506398</t>
+    <t>0xc0000ba960</t>
+  </si>
+  <si>
+    <t>0xc0000ba950</t>
+  </si>
+  <si>
+    <t>0xc0000ba970</t>
+  </si>
+  <si>
+    <t>0xc0000ba980</t>
+  </si>
+  <si>
+    <t>0xc0000ba990</t>
+  </si>
+  <si>
+    <t>0xc00042e5c0</t>
+  </si>
+  <si>
+    <t>0xc00042e5d8</t>
   </si>
   <si>
     <t>"09-22-12</t>
   </si>
   <si>
-    <t>0xc0005003e0</t>
-  </si>
-  <si>
-    <t>0xc0005003d0</t>
-  </si>
-  <si>
-    <t>0xc0005003f0</t>
-  </si>
-  <si>
-    <t>0xc000500400</t>
-  </si>
-  <si>
-    <t>0xc000500410</t>
-  </si>
-  <si>
-    <t>0xc0005063e0</t>
-  </si>
-  <si>
-    <t>0xc0005063f8</t>
+    <t>0xc0000ba9d0</t>
+  </si>
+  <si>
+    <t>0xc0000ba9c0</t>
+  </si>
+  <si>
+    <t>0xc0000ba9e0</t>
+  </si>
+  <si>
+    <t>0xc0000baa00</t>
+  </si>
+  <si>
+    <t>0xc0000baa20</t>
+  </si>
+  <si>
+    <t>0xc00042e670</t>
+  </si>
+  <si>
+    <t>0xc00042e698</t>
   </si>
   <si>
     <t>"09-22-13</t>
   </si>
   <si>
-    <t>0xc000500430</t>
-  </si>
-  <si>
-    <t>0xc000500420</t>
-  </si>
-  <si>
-    <t>0xc000500440</t>
-  </si>
-  <si>
-    <t>0xc000500450</t>
-  </si>
-  <si>
-    <t>0xc000500460</t>
-  </si>
-  <si>
-    <t>0xc000506430</t>
-  </si>
-  <si>
-    <t>0xc000506440</t>
+    <t>0xc0000baa50</t>
+  </si>
+  <si>
+    <t>0xc0000baa40</t>
+  </si>
+  <si>
+    <t>0xc0000baa60</t>
+  </si>
+  <si>
+    <t>0xc0000baa70</t>
+  </si>
+  <si>
+    <t>0xc0000baa80</t>
+  </si>
+  <si>
+    <t>0xc00042e6d0</t>
+  </si>
+  <si>
+    <t>0xc00042e6e0</t>
   </si>
   <si>
     <t>"09-22-14</t>
   </si>
   <si>
-    <t>0xc000500480</t>
-  </si>
-  <si>
-    <t>0xc000500470</t>
-  </si>
-  <si>
-    <t>0xc000500490</t>
-  </si>
-  <si>
-    <t>0xc0005004a0</t>
-  </si>
-  <si>
-    <t>0xc0005004b0</t>
-  </si>
-  <si>
-    <t>0xc000506490</t>
-  </si>
-  <si>
-    <t>0xc0005064a0</t>
+    <t>0xc0000baab0</t>
+  </si>
+  <si>
+    <t>0xc0000baaa0</t>
+  </si>
+  <si>
+    <t>0xc0000baac0</t>
+  </si>
+  <si>
+    <t>0xc0000baad0</t>
+  </si>
+  <si>
+    <t>0xc0000baae0</t>
+  </si>
+  <si>
+    <t>0xc00042e730</t>
+  </si>
+  <si>
+    <t>0xc00042e740</t>
   </si>
   <si>
     <t>"09-22-15</t>
   </si>
   <si>
-    <t>0xc0005004d0</t>
-  </si>
-  <si>
-    <t>0xc0005004c0</t>
-  </si>
-  <si>
-    <t>0xc0005004e0</t>
-  </si>
-  <si>
-    <t>0xc0005004f0</t>
-  </si>
-  <si>
-    <t>0xc000500500</t>
-  </si>
-  <si>
-    <t>0xc0005064d0</t>
-  </si>
-  <si>
-    <t>0xc0005064e8</t>
+    <t>0xc0000bab10</t>
+  </si>
+  <si>
+    <t>0xc0000bab00</t>
+  </si>
+  <si>
+    <t>0xc0000bab20</t>
+  </si>
+  <si>
+    <t>0xc0000bab30</t>
+  </si>
+  <si>
+    <t>0xc0000bab40</t>
+  </si>
+  <si>
+    <t>0xc00042e770</t>
+  </si>
+  <si>
+    <t>0xc00042e788</t>
   </si>
   <si>
     <t>"09-22-16</t>
   </si>
   <si>
-    <t>0xc000500520</t>
-  </si>
-  <si>
-    <t>0xc000500510</t>
-  </si>
-  <si>
-    <t>0xc000500530</t>
-  </si>
-  <si>
-    <t>0xc000500540</t>
-  </si>
-  <si>
-    <t>0xc000500550</t>
-  </si>
-  <si>
-    <t>0xc000506520</t>
-  </si>
-  <si>
-    <t>0xc000506530</t>
+    <t>0xc0000bab70</t>
+  </si>
+  <si>
+    <t>0xc0000bab60</t>
+  </si>
+  <si>
+    <t>0xc0000bab80</t>
+  </si>
+  <si>
+    <t>0xc0000bab90</t>
+  </si>
+  <si>
+    <t>0xc0000baba0</t>
+  </si>
+  <si>
+    <t>0xc00042e7c0</t>
+  </si>
+  <si>
+    <t>0xc00042e7d0</t>
   </si>
   <si>
     <t>"09-22-17</t>
   </si>
   <si>
-    <t>0xc000500570</t>
-  </si>
-  <si>
-    <t>0xc000500560</t>
-  </si>
-  <si>
-    <t>0xc000500580</t>
-  </si>
-  <si>
-    <t>0xc000500590</t>
-  </si>
-  <si>
-    <t>0xc0005005a0</t>
-  </si>
-  <si>
-    <t>0xc000506580</t>
-  </si>
-  <si>
-    <t>0xc000506598</t>
+    <t>0xc0000babd0</t>
+  </si>
+  <si>
+    <t>0xc0000babc0</t>
+  </si>
+  <si>
+    <t>0xc0000babf0</t>
+  </si>
+  <si>
+    <t>0xc0000bac10</t>
+  </si>
+  <si>
+    <t>0xc0000bac20</t>
+  </si>
+  <si>
+    <t>0xc00042e820</t>
+  </si>
+  <si>
+    <t>0xc00042e838</t>
   </si>
   <si>
     <t>"09-22-18</t>
   </si>
   <si>
-    <t>0xc0005005c0</t>
-  </si>
-  <si>
-    <t>0xc0005005b0</t>
-  </si>
-  <si>
-    <t>0xc0005005d0</t>
-  </si>
-  <si>
-    <t>0xc0005005e0</t>
-  </si>
-  <si>
-    <t>0xc0005005f0</t>
-  </si>
-  <si>
-    <t>0xc0005065d0</t>
-  </si>
-  <si>
-    <t>0xc0005065e0</t>
+    <t>0xc0000bac50</t>
+  </si>
+  <si>
+    <t>0xc0000bac40</t>
+  </si>
+  <si>
+    <t>0xc0000bac70</t>
+  </si>
+  <si>
+    <t>0xc0000bac90</t>
+  </si>
+  <si>
+    <t>0xc0000baca0</t>
+  </si>
+  <si>
+    <t>0xc00042e870</t>
+  </si>
+  <si>
+    <t>0xc00042e880</t>
   </si>
   <si>
     <t>"09-22-19</t>
   </si>
   <si>
-    <t>0xc000500610</t>
-  </si>
-  <si>
-    <t>0xc000500600</t>
-  </si>
-  <si>
-    <t>0xc000500620</t>
-  </si>
-  <si>
-    <t>0xc000500630</t>
-  </si>
-  <si>
-    <t>0xc000500640</t>
-  </si>
-  <si>
-    <t>0xc000506620</t>
-  </si>
-  <si>
-    <t>0xc000506630</t>
+    <t>0xc0000bace0</t>
+  </si>
+  <si>
+    <t>0xc0000bacd0</t>
+  </si>
+  <si>
+    <t>0xc0000bad10</t>
+  </si>
+  <si>
+    <t>0xc0000bad20</t>
+  </si>
+  <si>
+    <t>0xc0000bad30</t>
+  </si>
+  <si>
+    <t>0xc00042e8c0</t>
+  </si>
+  <si>
+    <t>0xc00042e8d0</t>
   </si>
   <si>
     <t>07-22-01</t>
   </si>
   <si>
-    <t>0xc000500660</t>
+    <t>0xc0000bad70</t>
   </si>
   <si>
     <t>W</t>
   </si>
   <si>
-    <t>0xc000500650</t>
-  </si>
-  <si>
-    <t>0xc000500670</t>
-  </si>
-  <si>
-    <t>0xc000500680</t>
-  </si>
-  <si>
-    <t>0xc000500690</t>
-  </si>
-  <si>
-    <t>0xc000506650</t>
+    <t>0xc0000bad50</t>
+  </si>
+  <si>
+    <t>0xc0000bad80</t>
+  </si>
+  <si>
+    <t>0xc0000bad90</t>
+  </si>
+  <si>
+    <t>0xc0000bada0</t>
+  </si>
+  <si>
+    <t>0xc00042e8f0</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>0xc000506660</t>
+    <t>0xc00042e900</t>
   </si>
   <si>
     <t>07-22-02</t>
   </si>
   <si>
-    <t>0xc0005006b0</t>
-  </si>
-  <si>
-    <t>0xc0005006a0</t>
-  </si>
-  <si>
-    <t>0xc0005006c0</t>
-  </si>
-  <si>
-    <t>0xc0005006d0</t>
-  </si>
-  <si>
-    <t>0xc0005006e0</t>
-  </si>
-  <si>
-    <t>0xc000506670</t>
-  </si>
-  <si>
-    <t>0xc000506680</t>
+    <t>0xc0000bade0</t>
+  </si>
+  <si>
+    <t>0xc0000badd0</t>
+  </si>
+  <si>
+    <t>0xc0000badf0</t>
+  </si>
+  <si>
+    <t>0xc0000bae00</t>
+  </si>
+  <si>
+    <t>0xc0000bae10</t>
+  </si>
+  <si>
+    <t>0xc00042e910</t>
+  </si>
+  <si>
+    <t>0xc00042e920</t>
   </si>
   <si>
     <t>07-22-03</t>
   </si>
   <si>
-    <t>0xc000500700</t>
-  </si>
-  <si>
-    <t>0xc0005006f0</t>
-  </si>
-  <si>
-    <t>0xc000500710</t>
-  </si>
-  <si>
-    <t>0xc000500720</t>
-  </si>
-  <si>
-    <t>0xc000500730</t>
-  </si>
-  <si>
-    <t>0xc000506690</t>
-  </si>
-  <si>
-    <t>0xc0005066a0</t>
+    <t>0xc0000bae40</t>
+  </si>
+  <si>
+    <t>0xc0000bae30</t>
+  </si>
+  <si>
+    <t>0xc0000bae60</t>
+  </si>
+  <si>
+    <t>0xc0000bae80</t>
+  </si>
+  <si>
+    <t>0xc0000bae90</t>
+  </si>
+  <si>
+    <t>0xc00042e930</t>
+  </si>
+  <si>
+    <t>0xc00042e940</t>
   </si>
   <si>
     <t>07-22-04</t>
   </si>
   <si>
-    <t>0xc000500750</t>
-  </si>
-  <si>
-    <t>0xc000500740</t>
-  </si>
-  <si>
-    <t>0xc000500760</t>
-  </si>
-  <si>
-    <t>0xc000500770</t>
-  </si>
-  <si>
-    <t>0xc000500780</t>
-  </si>
-  <si>
-    <t>0xc0005066c0</t>
-  </si>
-  <si>
-    <t>0xc0005066d0</t>
+    <t>0xc0000baec0</t>
+  </si>
+  <si>
+    <t>0xc0000baeb0</t>
+  </si>
+  <si>
+    <t>0xc0000baed0</t>
+  </si>
+  <si>
+    <t>0xc0000baee0</t>
+  </si>
+  <si>
+    <t>0xc0000baef0</t>
+  </si>
+  <si>
+    <t>0xc00042e960</t>
+  </si>
+  <si>
+    <t>0xc00042e970</t>
   </si>
   <si>
     <t>07-22-05</t>
   </si>
   <si>
-    <t>0xc0005007a0</t>
-  </si>
-  <si>
-    <t>0xc000500790</t>
-  </si>
-  <si>
-    <t>0xc0005007b0</t>
-  </si>
-  <si>
-    <t>0xc0005007c0</t>
-  </si>
-  <si>
-    <t>0xc0005007d0</t>
-  </si>
-  <si>
-    <t>0xc0005066e0</t>
-  </si>
-  <si>
-    <t>0xc0005066f0</t>
+    <t>0xc0000baf30</t>
+  </si>
+  <si>
+    <t>0xc0000baf20</t>
+  </si>
+  <si>
+    <t>0xc0000baf50</t>
+  </si>
+  <si>
+    <t>0xc0000baf60</t>
+  </si>
+  <si>
+    <t>0xc0000baf90</t>
+  </si>
+  <si>
+    <t>0xc00042e980</t>
+  </si>
+  <si>
+    <t>0xc00042e990</t>
   </si>
   <si>
     <t>07-22-06</t>
   </si>
   <si>
-    <t>0xc0005007f0</t>
-  </si>
-  <si>
-    <t>0xc0005007e0</t>
-  </si>
-  <si>
-    <t>0xc000500800</t>
-  </si>
-  <si>
-    <t>0xc000500810</t>
-  </si>
-  <si>
-    <t>0xc000500820</t>
-  </si>
-  <si>
-    <t>0xc000506710</t>
-  </si>
-  <si>
-    <t>0xc000506720</t>
+    <t>0xc0000bb070</t>
+  </si>
+  <si>
+    <t>0xc0000bb060</t>
+  </si>
+  <si>
+    <t>0xc0000bb080</t>
+  </si>
+  <si>
+    <t>0xc0000bb090</t>
+  </si>
+  <si>
+    <t>0xc0000bb0b0</t>
+  </si>
+  <si>
+    <t>0xc00042e9b0</t>
+  </si>
+  <si>
+    <t>0xc00042e9c0</t>
   </si>
   <si>
     <t>07-22-07</t>
   </si>
   <si>
-    <t>0xc000500840</t>
-  </si>
-  <si>
-    <t>0xc000500830</t>
-  </si>
-  <si>
-    <t>0xc000500850</t>
-  </si>
-  <si>
-    <t>0xc000500860</t>
-  </si>
-  <si>
-    <t>0xc000500870</t>
-  </si>
-  <si>
-    <t>0xc000506740</t>
-  </si>
-  <si>
-    <t>0xc000506750</t>
+    <t>0xc0000bb0f0</t>
+  </si>
+  <si>
+    <t>0xc0000bb0e0</t>
+  </si>
+  <si>
+    <t>0xc0000bb100</t>
+  </si>
+  <si>
+    <t>0xc0000bb110</t>
+  </si>
+  <si>
+    <t>0xc0000bb130</t>
+  </si>
+  <si>
+    <t>0xc00042e9e0</t>
+  </si>
+  <si>
+    <t>0xc00042e9f0</t>
   </si>
   <si>
     <t>07-22-08</t>
   </si>
   <si>
-    <t>0xc000500890</t>
-  </si>
-  <si>
-    <t>0xc000500880</t>
-  </si>
-  <si>
-    <t>0xc0005008a0</t>
-  </si>
-  <si>
-    <t>0xc0005008b0</t>
-  </si>
-  <si>
-    <t>0xc0005008c0</t>
-  </si>
-  <si>
-    <t>0xc000506780</t>
-  </si>
-  <si>
-    <t>0xc000506790</t>
+    <t>0xc0000bb170</t>
+  </si>
+  <si>
+    <t>0xc0000bb160</t>
+  </si>
+  <si>
+    <t>0xc0000bb180</t>
+  </si>
+  <si>
+    <t>0xc0000bb190</t>
+  </si>
+  <si>
+    <t>0xc0000bb1a0</t>
+  </si>
+  <si>
+    <t>0xc00042ea20</t>
+  </si>
+  <si>
+    <t>0xc00042ea30</t>
   </si>
   <si>
     <t>07-22-09</t>
   </si>
   <si>
-    <t>0xc0005008e0</t>
-  </si>
-  <si>
-    <t>0xc0005008d0</t>
-  </si>
-  <si>
-    <t>0xc0005008f0</t>
-  </si>
-  <si>
-    <t>0xc000500900</t>
-  </si>
-  <si>
-    <t>0xc000500910</t>
-  </si>
-  <si>
-    <t>0xc0005067b0</t>
-  </si>
-  <si>
-    <t>0xc0005067c0</t>
+    <t>0xc0000bb1e0</t>
+  </si>
+  <si>
+    <t>0xc0000bb1c0</t>
+  </si>
+  <si>
+    <t>0xc0000bb1f0</t>
+  </si>
+  <si>
+    <t>0xc0000bb200</t>
+  </si>
+  <si>
+    <t>0xc0000bb220</t>
+  </si>
+  <si>
+    <t>0xc00042ea60</t>
+  </si>
+  <si>
+    <t>0xc00042ea70</t>
   </si>
   <si>
     <t>07-22-10</t>
   </si>
   <si>
-    <t>0xc000500930</t>
-  </si>
-  <si>
-    <t>0xc000500920</t>
-  </si>
-  <si>
-    <t>0xc000500940</t>
-  </si>
-  <si>
-    <t>0xc000500950</t>
-  </si>
-  <si>
-    <t>0xc000500960</t>
-  </si>
-  <si>
-    <t>0xc0005067f0</t>
-  </si>
-  <si>
-    <t>0xc000506800</t>
+    <t>0xc0000bb250</t>
+  </si>
+  <si>
+    <t>0xc0000bb240</t>
+  </si>
+  <si>
+    <t>0xc0000bb260</t>
+  </si>
+  <si>
+    <t>0xc0000bb280</t>
+  </si>
+  <si>
+    <t>0xc0000bb290</t>
+  </si>
+  <si>
+    <t>0xc00042eaa0</t>
+  </si>
+  <si>
+    <t>0xc00042eab0</t>
   </si>
   <si>
     <t>07-22-11</t>
   </si>
   <si>
-    <t>0xc000500980</t>
-  </si>
-  <si>
-    <t>0xc000500970</t>
-  </si>
-  <si>
-    <t>0xc000500990</t>
-  </si>
-  <si>
-    <t>0xc0005009a0</t>
-  </si>
-  <si>
-    <t>0xc0005009b0</t>
-  </si>
-  <si>
-    <t>0xc000506830</t>
-  </si>
-  <si>
-    <t>0xc000506840</t>
+    <t>0xc0000bb2f0</t>
+  </si>
+  <si>
+    <t>0xc0000bb2d0</t>
+  </si>
+  <si>
+    <t>0xc0000bb300</t>
+  </si>
+  <si>
+    <t>0xc0000bb310</t>
+  </si>
+  <si>
+    <t>0xc0000bb320</t>
+  </si>
+  <si>
+    <t>0xc00042eae0</t>
+  </si>
+  <si>
+    <t>0xc00042eaf0</t>
   </si>
   <si>
     <t>07-22-12</t>
   </si>
   <si>
-    <t>0xc0005009d0</t>
-  </si>
-  <si>
-    <t>0xc0005009c0</t>
-  </si>
-  <si>
-    <t>0xc0005009e0</t>
-  </si>
-  <si>
-    <t>0xc0005009f0</t>
-  </si>
-  <si>
-    <t>0xc000500a00</t>
-  </si>
-  <si>
-    <t>0xc000506870</t>
-  </si>
-  <si>
-    <t>0xc000506880</t>
+    <t>0xc0000bb350</t>
+  </si>
+  <si>
+    <t>0xc0000bb340</t>
+  </si>
+  <si>
+    <t>0xc0000bb360</t>
+  </si>
+  <si>
+    <t>0xc0000bb370</t>
+  </si>
+  <si>
+    <t>0xc0000bb380</t>
+  </si>
+  <si>
+    <t>0xc00042eb20</t>
+  </si>
+  <si>
+    <t>0xc00042eb30</t>
   </si>
   <si>
     <t>07-22-13</t>
   </si>
   <si>
-    <t>0xc000500a20</t>
-  </si>
-  <si>
-    <t>0xc000500a10</t>
-  </si>
-  <si>
-    <t>0xc000500a30</t>
-  </si>
-  <si>
-    <t>0xc000500a40</t>
-  </si>
-  <si>
-    <t>0xc000500a50</t>
-  </si>
-  <si>
-    <t>0xc0005068a0</t>
-  </si>
-  <si>
-    <t>0xc0005068b0</t>
+    <t>0xc0000bb3b0</t>
+  </si>
+  <si>
+    <t>0xc0000bb3a0</t>
+  </si>
+  <si>
+    <t>0xc0000bb3c0</t>
+  </si>
+  <si>
+    <t>0xc0000bb3d0</t>
+  </si>
+  <si>
+    <t>0xc0000bb3e0</t>
+  </si>
+  <si>
+    <t>0xc00042eb50</t>
+  </si>
+  <si>
+    <t>0xc00042eb60</t>
   </si>
   <si>
     <t>07-22-14</t>
   </si>
   <si>
-    <t>0xc000500a70</t>
-  </si>
-  <si>
-    <t>0xc000500a60</t>
-  </si>
-  <si>
-    <t>0xc000500a80</t>
-  </si>
-  <si>
-    <t>0xc000500a90</t>
-  </si>
-  <si>
-    <t>0xc000500aa0</t>
-  </si>
-  <si>
-    <t>0xc0005068e0</t>
-  </si>
-  <si>
-    <t>0xc0005068f0</t>
+    <t>0xc0000bb410</t>
+  </si>
+  <si>
+    <t>0xc0000bb400</t>
+  </si>
+  <si>
+    <t>0xc0000bb420</t>
+  </si>
+  <si>
+    <t>0xc0000bb430</t>
+  </si>
+  <si>
+    <t>0xc0000bb440</t>
+  </si>
+  <si>
+    <t>0xc00042eb90</t>
+  </si>
+  <si>
+    <t>0xc00042eba0</t>
   </si>
   <si>
     <t>07-22-15</t>
   </si>
   <si>
-    <t>0xc000500ac0</t>
-  </si>
-  <si>
-    <t>0xc000500ab0</t>
-  </si>
-  <si>
-    <t>0xc000500ad0</t>
-  </si>
-  <si>
-    <t>0xc000500ae0</t>
-  </si>
-  <si>
-    <t>0xc000500af0</t>
-  </si>
-  <si>
-    <t>0xc000506910</t>
-  </si>
-  <si>
-    <t>0xc000506920</t>
+    <t>0xc0000bb470</t>
+  </si>
+  <si>
+    <t>0xc0000bb460</t>
+  </si>
+  <si>
+    <t>0xc0000bb480</t>
+  </si>
+  <si>
+    <t>0xc0000bb490</t>
+  </si>
+  <si>
+    <t>0xc0000bb4a0</t>
+  </si>
+  <si>
+    <t>0xc00042ebc0</t>
+  </si>
+  <si>
+    <t>0xc00042ebd0</t>
   </si>
   <si>
     <t>07-22-16</t>
   </si>
   <si>
-    <t>0xc000500b10</t>
-  </si>
-  <si>
-    <t>0xc000500b00</t>
-  </si>
-  <si>
-    <t>0xc000500b20</t>
-  </si>
-  <si>
-    <t>0xc000500b30</t>
-  </si>
-  <si>
-    <t>0xc000500b40</t>
-  </si>
-  <si>
-    <t>0xc000506940</t>
-  </si>
-  <si>
-    <t>0xc000506950</t>
+    <t>0xc0000bb4d0</t>
+  </si>
+  <si>
+    <t>0xc0000bb4c0</t>
+  </si>
+  <si>
+    <t>0xc0000bb4e0</t>
+  </si>
+  <si>
+    <t>0xc0000bb4f0</t>
+  </si>
+  <si>
+    <t>0xc0000bb500</t>
+  </si>
+  <si>
+    <t>0xc00042ec00</t>
+  </si>
+  <si>
+    <t>0xc00042ec10</t>
   </si>
   <si>
     <t>07-22-17</t>
   </si>
   <si>
-    <t>0xc000500b60</t>
-  </si>
-  <si>
-    <t>0xc000500b50</t>
-  </si>
-  <si>
-    <t>0xc000500ba0</t>
-  </si>
-  <si>
-    <t>0xc000500c00</t>
-  </si>
-  <si>
-    <t>0xc000500c10</t>
-  </si>
-  <si>
-    <t>0xc000506980</t>
-  </si>
-  <si>
-    <t>0xc000506990</t>
+    <t>0xc0000bb530</t>
+  </si>
+  <si>
+    <t>0xc0000bb520</t>
+  </si>
+  <si>
+    <t>0xc0000bb540</t>
+  </si>
+  <si>
+    <t>0xc0000bb550</t>
+  </si>
+  <si>
+    <t>0xc0000bb560</t>
+  </si>
+  <si>
+    <t>0xc00042ec40</t>
+  </si>
+  <si>
+    <t>0xc00042ec50</t>
   </si>
   <si>
     <t>07-22-18</t>
   </si>
   <si>
-    <t>0xc000500c40</t>
-  </si>
-  <si>
-    <t>0xc000500c30</t>
-  </si>
-  <si>
-    <t>0xc000500c50</t>
-  </si>
-  <si>
-    <t>0xc000500c60</t>
-  </si>
-  <si>
-    <t>0xc000500c70</t>
-  </si>
-  <si>
-    <t>0xc0005069c0</t>
-  </si>
-  <si>
-    <t>0xc0005069d0</t>
+    <t>0xc0000bb590</t>
+  </si>
+  <si>
+    <t>0xc0000bb580</t>
+  </si>
+  <si>
+    <t>0xc0000bb5a0</t>
+  </si>
+  <si>
+    <t>0xc0000bb5b0</t>
+  </si>
+  <si>
+    <t>0xc0000bb5c0</t>
+  </si>
+  <si>
+    <t>0xc00042ec80</t>
+  </si>
+  <si>
+    <t>0xc00042ec90</t>
   </si>
   <si>
     <t>07-22-19</t>
   </si>
   <si>
-    <t>0xc000500c90</t>
-  </si>
-  <si>
-    <t>0xc000500c80</t>
-  </si>
-  <si>
-    <t>0xc000500ca0</t>
-  </si>
-  <si>
-    <t>0xc000500cb0</t>
-  </si>
-  <si>
-    <t>0xc000500cc0</t>
-  </si>
-  <si>
-    <t>0xc0005069f0</t>
-  </si>
-  <si>
-    <t>0xc000506a00</t>
+    <t>0xc0000bb5f0</t>
+  </si>
+  <si>
+    <t>0xc0000bb5e0</t>
+  </si>
+  <si>
+    <t>0xc0000bb610</t>
+  </si>
+  <si>
+    <t>0xc0000bb620</t>
+  </si>
+  <si>
+    <t>0xc0000bb630</t>
+  </si>
+  <si>
+    <t>0xc00042ecb0</t>
+  </si>
+  <si>
+    <t>0xc00042ecc0</t>
   </si>
   <si>
     <t>07-22-20</t>
   </si>
   <si>
-    <t>0xc000500ce0</t>
-  </si>
-  <si>
-    <t>0xc000500cd0</t>
-  </si>
-  <si>
-    <t>0xc000500cf0</t>
-  </si>
-  <si>
-    <t>0xc000500d00</t>
-  </si>
-  <si>
-    <t>0xc000500d10</t>
-  </si>
-  <si>
-    <t>0xc000506a30</t>
-  </si>
-  <si>
-    <t>0xc000506a40</t>
+    <t>0xc0000bb670</t>
+  </si>
+  <si>
+    <t>0xc0000bb650</t>
+  </si>
+  <si>
+    <t>0xc0000bb680</t>
+  </si>
+  <si>
+    <t>0xc0000bb690</t>
+  </si>
+  <si>
+    <t>0xc0000bb6a0</t>
+  </si>
+  <si>
+    <t>0xc00042ecf0</t>
+  </si>
+  <si>
+    <t>0xc00042ed00</t>
   </si>
   <si>
     <t>07-22-21</t>
   </si>
   <si>
-    <t>0xc000500d30</t>
-  </si>
-  <si>
-    <t>0xc000500d20</t>
-  </si>
-  <si>
-    <t>0xc000500d40</t>
-  </si>
-  <si>
-    <t>0xc000500d50</t>
-  </si>
-  <si>
-    <t>0xc000500d60</t>
-  </si>
-  <si>
-    <t>0xc000506a70</t>
-  </si>
-  <si>
-    <t>0xc000506a80</t>
+    <t>0xc0000bb6d0</t>
+  </si>
+  <si>
+    <t>0xc0000bb6c0</t>
+  </si>
+  <si>
+    <t>0xc0000bb6e0</t>
+  </si>
+  <si>
+    <t>0xc0000bb6f0</t>
+  </si>
+  <si>
+    <t>0xc0000bb700</t>
+  </si>
+  <si>
+    <t>0xc00042ed30</t>
+  </si>
+  <si>
+    <t>0xc00042ed40</t>
   </si>
   <si>
     <t>08-22-01</t>
   </si>
   <si>
-    <t>0xc000500d80</t>
-  </si>
-  <si>
-    <t>0xc000500d70</t>
-  </si>
-  <si>
-    <t>0xc000500d90</t>
-  </si>
-  <si>
-    <t>0xc000500da0</t>
-  </si>
-  <si>
-    <t>0xc000500db0</t>
-  </si>
-  <si>
-    <t>0xc000506aa0</t>
-  </si>
-  <si>
-    <t>0xc000506ab0</t>
+    <t>0xc0000bb730</t>
+  </si>
+  <si>
+    <t>0xc0000bb720</t>
+  </si>
+  <si>
+    <t>0xc0000bb740</t>
+  </si>
+  <si>
+    <t>0xc0000bb750</t>
+  </si>
+  <si>
+    <t>0xc0000bb760</t>
+  </si>
+  <si>
+    <t>0xc00042ed70</t>
+  </si>
+  <si>
+    <t>0xc00042ed80</t>
   </si>
   <si>
     <t>08-22-02</t>
   </si>
   <si>
-    <t>0xc000500dd0</t>
-  </si>
-  <si>
-    <t>0xc000500dc0</t>
-  </si>
-  <si>
-    <t>0xc000500de0</t>
-  </si>
-  <si>
-    <t>0xc000500df0</t>
-  </si>
-  <si>
-    <t>0xc000500e00</t>
-  </si>
-  <si>
-    <t>0xc000506ad0</t>
-  </si>
-  <si>
-    <t>0xc000506ae0</t>
+    <t>0xc0000bb7a0</t>
+  </si>
+  <si>
+    <t>0xc0000bb780</t>
+  </si>
+  <si>
+    <t>0xc0000bb7b0</t>
+  </si>
+  <si>
+    <t>0xc0000bb7d0</t>
+  </si>
+  <si>
+    <t>0xc0000bb7e0</t>
+  </si>
+  <si>
+    <t>0xc00042eda0</t>
+  </si>
+  <si>
+    <t>0xc00042edb0</t>
   </si>
   <si>
     <t>08-22-03</t>
   </si>
   <si>
-    <t>0xc000500e20</t>
-  </si>
-  <si>
-    <t>0xc000500e10</t>
-  </si>
-  <si>
-    <t>0xc000500e30</t>
-  </si>
-  <si>
-    <t>0xc000500e40</t>
-  </si>
-  <si>
-    <t>0xc000500e50</t>
-  </si>
-  <si>
-    <t>0xc000506af8</t>
-  </si>
-  <si>
-    <t>0xc000506b08</t>
+    <t>0xc0000bb820</t>
+  </si>
+  <si>
+    <t>0xc0000bb810</t>
+  </si>
+  <si>
+    <t>0xc0000bb830</t>
+  </si>
+  <si>
+    <t>0xc0000bb840</t>
+  </si>
+  <si>
+    <t>0xc0000bb850</t>
+  </si>
+  <si>
+    <t>0xc00042edc8</t>
+  </si>
+  <si>
+    <t>0xc00042edd8</t>
   </si>
   <si>
     <t>08-22-04</t>
   </si>
   <si>
-    <t>0xc000500e70</t>
-  </si>
-  <si>
-    <t>0xc000500e60</t>
-  </si>
-  <si>
-    <t>0xc000500e80</t>
-  </si>
-  <si>
-    <t>0xc000500e90</t>
-  </si>
-  <si>
-    <t>0xc000500ea0</t>
-  </si>
-  <si>
-    <t>0xc000506b30</t>
-  </si>
-  <si>
-    <t>0xc000506b40</t>
+    <t>0xc0000bb880</t>
+  </si>
+  <si>
+    <t>0xc0000bb870</t>
+  </si>
+  <si>
+    <t>0xc0000bb890</t>
+  </si>
+  <si>
+    <t>0xc0000bb8a0</t>
+  </si>
+  <si>
+    <t>0xc0000bb8b0</t>
+  </si>
+  <si>
+    <t>0xc00042ee00</t>
+  </si>
+  <si>
+    <t>0xc00042ee10</t>
   </si>
   <si>
     <t>08-22-05</t>
   </si>
   <si>
-    <t>0xc000500ec0</t>
-  </si>
-  <si>
-    <t>0xc000500eb0</t>
-  </si>
-  <si>
-    <t>0xc000500ed0</t>
-  </si>
-  <si>
-    <t>0xc000500ee0</t>
-  </si>
-  <si>
-    <t>0xc000500ef0</t>
-  </si>
-  <si>
-    <t>0xc000506b58</t>
-  </si>
-  <si>
-    <t>0xc000506b68</t>
+    <t>0xc0000bb8f0</t>
+  </si>
+  <si>
+    <t>0xc0000bb8e0</t>
+  </si>
+  <si>
+    <t>0xc0000bb920</t>
+  </si>
+  <si>
+    <t>0xc0000bb930</t>
+  </si>
+  <si>
+    <t>0xc0000bb940</t>
+  </si>
+  <si>
+    <t>0xc00042ee28</t>
+  </si>
+  <si>
+    <t>0xc00042ee38</t>
   </si>
   <si>
     <t>08-22-06</t>
   </si>
   <si>
-    <t>0xc000500f10</t>
-  </si>
-  <si>
-    <t>0xc000500f00</t>
-  </si>
-  <si>
-    <t>0xc000500f20</t>
-  </si>
-  <si>
-    <t>0xc000500f30</t>
-  </si>
-  <si>
-    <t>0xc000500f40</t>
-  </si>
-  <si>
-    <t>0xc000506b80</t>
-  </si>
-  <si>
-    <t>0xc000506b90</t>
+    <t>0xc0000bb980</t>
+  </si>
+  <si>
+    <t>0xc0000bb970</t>
+  </si>
+  <si>
+    <t>0xc0000bb990</t>
+  </si>
+  <si>
+    <t>0xc0000bb9a0</t>
+  </si>
+  <si>
+    <t>0xc0000bb9b0</t>
+  </si>
+  <si>
+    <t>0xc00042ee50</t>
+  </si>
+  <si>
+    <t>0xc00042ee60</t>
   </si>
   <si>
     <t>08-22-07</t>
   </si>
   <si>
-    <t>0xc000500f60</t>
-  </si>
-  <si>
-    <t>0xc000500f50</t>
-  </si>
-  <si>
-    <t>0xc000500f70</t>
-  </si>
-  <si>
-    <t>0xc000500f80</t>
-  </si>
-  <si>
-    <t>0xc000500f90</t>
-  </si>
-  <si>
-    <t>0xc000506bb0</t>
-  </si>
-  <si>
-    <t>0xc000506bc0</t>
+    <t>0xc0000bb9e0</t>
+  </si>
+  <si>
+    <t>0xc0000bb9d0</t>
+  </si>
+  <si>
+    <t>0xc0000bb9f0</t>
+  </si>
+  <si>
+    <t>0xc0000bba00</t>
+  </si>
+  <si>
+    <t>0xc0000bba10</t>
+  </si>
+  <si>
+    <t>0xc00042ee80</t>
+  </si>
+  <si>
+    <t>0xc00042ee90</t>
   </si>
   <si>
     <t>08-22-08</t>
   </si>
   <si>
-    <t>0xc000500fb0</t>
-  </si>
-  <si>
-    <t>0xc000500fa0</t>
-  </si>
-  <si>
-    <t>0xc000500fc0</t>
-  </si>
-  <si>
-    <t>0xc000500fd0</t>
-  </si>
-  <si>
-    <t>0xc000500fe0</t>
-  </si>
-  <si>
-    <t>0xc000506be0</t>
-  </si>
-  <si>
-    <t>0xc000506bf0</t>
+    <t>0xc0000bba50</t>
+  </si>
+  <si>
+    <t>0xc0000bba30</t>
+  </si>
+  <si>
+    <t>0xc0000bba60</t>
+  </si>
+  <si>
+    <t>0xc0000bba70</t>
+  </si>
+  <si>
+    <t>0xc0000bba80</t>
+  </si>
+  <si>
+    <t>0xc00042eeb0</t>
+  </si>
+  <si>
+    <t>0xc00042eec0</t>
   </si>
   <si>
     <t>08-22-09</t>
   </si>
   <si>
-    <t>0xc000501000</t>
-  </si>
-  <si>
-    <t>0xc000500ff0</t>
-  </si>
-  <si>
-    <t>0xc000501010</t>
-  </si>
-  <si>
-    <t>0xc000501020</t>
-  </si>
-  <si>
-    <t>0xc000501030</t>
-  </si>
-  <si>
-    <t>0xc000506c10</t>
-  </si>
-  <si>
-    <t>0xc000506c20</t>
+    <t>0xc0000bbab0</t>
+  </si>
+  <si>
+    <t>0xc0000bbaa0</t>
+  </si>
+  <si>
+    <t>0xc0000bbac0</t>
+  </si>
+  <si>
+    <t>0xc0000bbad0</t>
+  </si>
+  <si>
+    <t>0xc0000bbae0</t>
+  </si>
+  <si>
+    <t>0xc00042eee0</t>
+  </si>
+  <si>
+    <t>0xc00042eef0</t>
   </si>
   <si>
     <t>08-22-10</t>
   </si>
   <si>
-    <t>0xc000501050</t>
-  </si>
-  <si>
-    <t>0xc000501040</t>
-  </si>
-  <si>
-    <t>0xc000501060</t>
-  </si>
-  <si>
-    <t>0xc000501070</t>
-  </si>
-  <si>
-    <t>0xc000501080</t>
-  </si>
-  <si>
-    <t>0xc000506c40</t>
-  </si>
-  <si>
-    <t>0xc000506c50</t>
+    <t>0xc0000bbb10</t>
+  </si>
+  <si>
+    <t>0xc0000bbb00</t>
+  </si>
+  <si>
+    <t>0xc0000bbb20</t>
+  </si>
+  <si>
+    <t>0xc0000bbb30</t>
+  </si>
+  <si>
+    <t>0xc0000bbb40</t>
+  </si>
+  <si>
+    <t>0xc00042ef10</t>
+  </si>
+  <si>
+    <t>0xc00042ef20</t>
   </si>
   <si>
     <t>08-22-11</t>
   </si>
   <si>
-    <t>0xc0005010a0</t>
-  </si>
-  <si>
-    <t>0xc000501090</t>
-  </si>
-  <si>
-    <t>0xc0005010b0</t>
-  </si>
-  <si>
-    <t>0xc0005010c0</t>
-  </si>
-  <si>
-    <t>0xc0005010d0</t>
-  </si>
-  <si>
-    <t>0xc000506c70</t>
-  </si>
-  <si>
-    <t>0xc000506c80</t>
+    <t>0xc0000bbb70</t>
+  </si>
+  <si>
+    <t>0xc0000bbb60</t>
+  </si>
+  <si>
+    <t>0xc0000bbb80</t>
+  </si>
+  <si>
+    <t>0xc0000bbb90</t>
+  </si>
+  <si>
+    <t>0xc0000bbba0</t>
+  </si>
+  <si>
+    <t>0xc00042ef40</t>
+  </si>
+  <si>
+    <t>0xc00042ef50</t>
   </si>
   <si>
     <t>08-22-12</t>
   </si>
   <si>
-    <t>0xc0005010f0</t>
-  </si>
-  <si>
-    <t>0xc0005010e0</t>
-  </si>
-  <si>
-    <t>0xc000501100</t>
-  </si>
-  <si>
-    <t>0xc000501110</t>
-  </si>
-  <si>
-    <t>0xc000501120</t>
-  </si>
-  <si>
-    <t>0xc000506ca0</t>
-  </si>
-  <si>
-    <t>0xc000506cb0</t>
+    <t>0xc0000bbbd0</t>
+  </si>
+  <si>
+    <t>0xc0000bbbc0</t>
+  </si>
+  <si>
+    <t>0xc0000bbbe0</t>
+  </si>
+  <si>
+    <t>0xc0000bbbf0</t>
+  </si>
+  <si>
+    <t>0xc0000bbc00</t>
+  </si>
+  <si>
+    <t>0xc00042ef70</t>
+  </si>
+  <si>
+    <t>0xc00042ef80</t>
   </si>
   <si>
     <t>08-22-13</t>
   </si>
   <si>
-    <t>0xc000501140</t>
-  </si>
-  <si>
-    <t>0xc000501130</t>
-  </si>
-  <si>
-    <t>0xc000501150</t>
-  </si>
-  <si>
-    <t>0xc000501160</t>
-  </si>
-  <si>
-    <t>0xc000501170</t>
-  </si>
-  <si>
-    <t>0xc000506cd0</t>
-  </si>
-  <si>
-    <t>0xc000506ce0</t>
+    <t>0xc0000bbc30</t>
+  </si>
+  <si>
+    <t>0xc0000bbc20</t>
+  </si>
+  <si>
+    <t>0xc0000bbc40</t>
+  </si>
+  <si>
+    <t>0xc0000bbc50</t>
+  </si>
+  <si>
+    <t>0xc0000bbc60</t>
+  </si>
+  <si>
+    <t>0xc00042efa0</t>
+  </si>
+  <si>
+    <t>0xc00042efb0</t>
   </si>
   <si>
     <t>08-22-14</t>
   </si>
   <si>
-    <t>0xc000501190</t>
-  </si>
-  <si>
-    <t>0xc000501180</t>
-  </si>
-  <si>
-    <t>0xc0005011a0</t>
-  </si>
-  <si>
-    <t>0xc0005011b0</t>
-  </si>
-  <si>
-    <t>0xc0005011c0</t>
-  </si>
-  <si>
-    <t>0xc000506d00</t>
-  </si>
-  <si>
-    <t>0xc000506d10</t>
+    <t>0xc0000bbc90</t>
+  </si>
+  <si>
+    <t>0xc0000bbc80</t>
+  </si>
+  <si>
+    <t>0xc0000bbca0</t>
+  </si>
+  <si>
+    <t>0xc0000bbcb0</t>
+  </si>
+  <si>
+    <t>0xc0000bbcc0</t>
+  </si>
+  <si>
+    <t>0xc00042efd0</t>
+  </si>
+  <si>
+    <t>0xc00042efe0</t>
   </si>
   <si>
     <t>08-22-15</t>
   </si>
   <si>
-    <t>0xc0005011e0</t>
-  </si>
-  <si>
-    <t>0xc0005011d0</t>
-  </si>
-  <si>
-    <t>0xc0005011f0</t>
-  </si>
-  <si>
-    <t>0xc000501200</t>
-  </si>
-  <si>
-    <t>0xc000501210</t>
-  </si>
-  <si>
-    <t>0xc000506d30</t>
-  </si>
-  <si>
-    <t>0xc000506d40</t>
+    <t>0xc0000bbcf0</t>
+  </si>
+  <si>
+    <t>0xc0000bbce0</t>
+  </si>
+  <si>
+    <t>0xc0000bbd00</t>
+  </si>
+  <si>
+    <t>0xc0000bbd10</t>
+  </si>
+  <si>
+    <t>0xc0000bbd20</t>
+  </si>
+  <si>
+    <t>0xc00042f010</t>
+  </si>
+  <si>
+    <t>0xc00042f020</t>
   </si>
   <si>
     <t>08-22-16</t>
   </si>
   <si>
-    <t>0xc000501230</t>
-  </si>
-  <si>
-    <t>0xc000501220</t>
-  </si>
-  <si>
-    <t>0xc000501240</t>
-  </si>
-  <si>
-    <t>0xc000501250</t>
-  </si>
-  <si>
-    <t>0xc000501260</t>
-  </si>
-  <si>
-    <t>0xc000506d60</t>
-  </si>
-  <si>
-    <t>0xc000506d70</t>
+    <t>0xc0000bbd50</t>
+  </si>
+  <si>
+    <t>0xc0000bbd40</t>
+  </si>
+  <si>
+    <t>0xc0000bbd60</t>
+  </si>
+  <si>
+    <t>0xc0000bbd70</t>
+  </si>
+  <si>
+    <t>0xc0000bbd80</t>
+  </si>
+  <si>
+    <t>0xc00042f040</t>
+  </si>
+  <si>
+    <t>0xc00042f050</t>
   </si>
   <si>
     <t>08-22-17</t>
   </si>
   <si>
-    <t>0xc000501280</t>
-  </si>
-  <si>
-    <t>0xc000501270</t>
-  </si>
-  <si>
-    <t>0xc000501290</t>
-  </si>
-  <si>
-    <t>0xc0005012a0</t>
-  </si>
-  <si>
-    <t>0xc0005012b0</t>
-  </si>
-  <si>
-    <t>0xc000506d90</t>
-  </si>
-  <si>
-    <t>0xc000506da0</t>
+    <t>0xc0000bbdb0</t>
+  </si>
+  <si>
+    <t>0xc0000bbda0</t>
+  </si>
+  <si>
+    <t>0xc0000bbdc0</t>
+  </si>
+  <si>
+    <t>0xc0000bbdd0</t>
+  </si>
+  <si>
+    <t>0xc0000bbde0</t>
+  </si>
+  <si>
+    <t>0xc00042f070</t>
+  </si>
+  <si>
+    <t>0xc00042f080</t>
   </si>
   <si>
     <t>08-22-18</t>
   </si>
   <si>
-    <t>0xc0005012d0</t>
-  </si>
-  <si>
-    <t>0xc0005012c0</t>
-  </si>
-  <si>
-    <t>0xc0005012e0</t>
-  </si>
-  <si>
-    <t>0xc0005012f0</t>
-  </si>
-  <si>
-    <t>0xc000501300</t>
-  </si>
-  <si>
-    <t>0xc000506db8</t>
-  </si>
-  <si>
-    <t>0xc000506dd8</t>
+    <t>0xc0000bbe10</t>
+  </si>
+  <si>
+    <t>0xc0000bbe00</t>
+  </si>
+  <si>
+    <t>0xc0000bbe20</t>
+  </si>
+  <si>
+    <t>0xc0000bbe30</t>
+  </si>
+  <si>
+    <t>0xc0000bbe40</t>
+  </si>
+  <si>
+    <t>0xc00042f098</t>
+  </si>
+  <si>
+    <t>0xc00042f0b8</t>
   </si>
   <si>
     <t>08-22-19</t>
   </si>
   <si>
-    <t>0xc000501320</t>
-  </si>
-  <si>
-    <t>0xc000501310</t>
-  </si>
-  <si>
-    <t>0xc000501330</t>
-  </si>
-  <si>
-    <t>0xc000501340</t>
-  </si>
-  <si>
-    <t>0xc000501350</t>
-  </si>
-  <si>
-    <t>0xc000506e00</t>
-  </si>
-  <si>
-    <t>0xc000506e10</t>
+    <t>0xc0000bbe70</t>
+  </si>
+  <si>
+    <t>0xc0000bbe60</t>
+  </si>
+  <si>
+    <t>0xc0000bbe80</t>
+  </si>
+  <si>
+    <t>0xc0000bbe90</t>
+  </si>
+  <si>
+    <t>0xc0000bbea0</t>
+  </si>
+  <si>
+    <t>0xc00042f0e0</t>
+  </si>
+  <si>
+    <t>0xc00042f0f0</t>
   </si>
   <si>
     <t>08-22-20</t>
   </si>
   <si>
-    <t>0xc000501370</t>
-  </si>
-  <si>
-    <t>0xc000501360</t>
-  </si>
-  <si>
-    <t>0xc000501380</t>
-  </si>
-  <si>
-    <t>0xc000501390</t>
-  </si>
-  <si>
-    <t>0xc0005013a0</t>
-  </si>
-  <si>
-    <t>0xc000506e30</t>
-  </si>
-  <si>
-    <t>0xc000506e40</t>
+    <t>0xc0000bbed0</t>
+  </si>
+  <si>
+    <t>0xc0000bbec0</t>
+  </si>
+  <si>
+    <t>0xc0000bbee0</t>
+  </si>
+  <si>
+    <t>0xc0000bbef0</t>
+  </si>
+  <si>
+    <t>0xc0000bbf00</t>
+  </si>
+  <si>
+    <t>0xc00042f110</t>
+  </si>
+  <si>
+    <t>0xc00042f120</t>
   </si>
   <si>
     <t>08-22-21</t>
   </si>
   <si>
-    <t>0xc0005013c0</t>
-  </si>
-  <si>
-    <t>0xc0005013b0</t>
-  </si>
-  <si>
-    <t>0xc0005013d0</t>
-  </si>
-  <si>
-    <t>0xc0005013e0</t>
-  </si>
-  <si>
-    <t>0xc0005013f0</t>
-  </si>
-  <si>
-    <t>0xc000506e58</t>
-  </si>
-  <si>
-    <t>0xc000506e68</t>
+    <t>0xc0000bbf30</t>
+  </si>
+  <si>
+    <t>0xc0000bbf20</t>
+  </si>
+  <si>
+    <t>0xc0000bbf40</t>
+  </si>
+  <si>
+    <t>0xc0000bbf50</t>
+  </si>
+  <si>
+    <t>0xc0000bbf60</t>
+  </si>
+  <si>
+    <t>0xc00042f138</t>
+  </si>
+  <si>
+    <t>0xc00042f148</t>
   </si>
   <si>
     <t>08-22-22</t>
   </si>
   <si>
-    <t>0xc000501410</t>
-  </si>
-  <si>
-    <t>0xc000501400</t>
-  </si>
-  <si>
-    <t>0xc000501420</t>
-  </si>
-  <si>
-    <t>0xc000501430</t>
-  </si>
-  <si>
-    <t>0xc000501440</t>
-  </si>
-  <si>
-    <t>0xc000506e90</t>
-  </si>
-  <si>
-    <t>0xc000506ea0</t>
+    <t>0xc0000bbf90</t>
+  </si>
+  <si>
+    <t>0xc0000bbf80</t>
+  </si>
+  <si>
+    <t>0xc0000bbfa0</t>
+  </si>
+  <si>
+    <t>0xc0000bbfb0</t>
+  </si>
+  <si>
+    <t>0xc0000bbfc0</t>
+  </si>
+  <si>
+    <t>0xc00042f170</t>
+  </si>
+  <si>
+    <t>0xc00042f180</t>
   </si>
   <si>
     <t>09-22-02</t>
   </si>
   <si>
-    <t>0xc000501460</t>
-  </si>
-  <si>
-    <t>0xc000501450</t>
-  </si>
-  <si>
-    <t>0xc000501470</t>
-  </si>
-  <si>
-    <t>0xc000501480</t>
-  </si>
-  <si>
-    <t>0xc000501490</t>
-  </si>
-  <si>
-    <t>0xc000506ed0</t>
-  </si>
-  <si>
-    <t>0xc000506ee0</t>
+    <t>0xc0000bbff0</t>
+  </si>
+  <si>
+    <t>0xc0000bbfe0</t>
+  </si>
+  <si>
+    <t>0xc000200000</t>
+  </si>
+  <si>
+    <t>0xc000200010</t>
+  </si>
+  <si>
+    <t>0xc000200020</t>
+  </si>
+  <si>
+    <t>0xc00042f1b0</t>
+  </si>
+  <si>
+    <t>0xc00042f1c0</t>
   </si>
   <si>
     <t>10-22-01</t>
   </si>
   <si>
-    <t>0xc0005014b0</t>
-  </si>
-  <si>
-    <t>0xc0005014a0</t>
-  </si>
-  <si>
-    <t>0xc0005014c0</t>
-  </si>
-  <si>
-    <t>0xc0005014d0</t>
-  </si>
-  <si>
-    <t>0xc0005014e0</t>
-  </si>
-  <si>
-    <t>0xc000506f00</t>
-  </si>
-  <si>
-    <t>0xc000506f10</t>
+    <t>0xc000200050</t>
+  </si>
+  <si>
+    <t>0xc000200040</t>
+  </si>
+  <si>
+    <t>0xc000200060</t>
+  </si>
+  <si>
+    <t>0xc000200070</t>
+  </si>
+  <si>
+    <t>0xc000200080</t>
+  </si>
+  <si>
+    <t>0xc00042f1e0</t>
+  </si>
+  <si>
+    <t>0xc00042f1f0</t>
   </si>
   <si>
     <t>10-22-02</t>
   </si>
   <si>
-    <t>0xc000501500</t>
-  </si>
-  <si>
-    <t>0xc0005014f0</t>
-  </si>
-  <si>
-    <t>0xc000501510</t>
-  </si>
-  <si>
-    <t>0xc000501520</t>
-  </si>
-  <si>
-    <t>0xc000501530</t>
-  </si>
-  <si>
-    <t>0xc000506f30</t>
-  </si>
-  <si>
-    <t>0xc000506f40</t>
+    <t>0xc0002000b0</t>
+  </si>
+  <si>
+    <t>0xc0002000a0</t>
+  </si>
+  <si>
+    <t>0xc0002000c0</t>
+  </si>
+  <si>
+    <t>0xc0002000d0</t>
+  </si>
+  <si>
+    <t>0xc0002000e0</t>
+  </si>
+  <si>
+    <t>0xc00042f210</t>
+  </si>
+  <si>
+    <t>0xc00042f220</t>
   </si>
   <si>
     <t>10-22-03</t>
   </si>
   <si>
-    <t>0xc000501550</t>
-  </si>
-  <si>
-    <t>0xc000501540</t>
-  </si>
-  <si>
-    <t>0xc000501560</t>
-  </si>
-  <si>
-    <t>0xc000501570</t>
-  </si>
-  <si>
-    <t>0xc000501580</t>
-  </si>
-  <si>
-    <t>0xc000506f58</t>
-  </si>
-  <si>
-    <t>0xc000506f78</t>
+    <t>0xc000200110</t>
+  </si>
+  <si>
+    <t>0xc000200100</t>
+  </si>
+  <si>
+    <t>0xc000200120</t>
+  </si>
+  <si>
+    <t>0xc000200130</t>
+  </si>
+  <si>
+    <t>0xc000200140</t>
+  </si>
+  <si>
+    <t>0xc00042f238</t>
+  </si>
+  <si>
+    <t>0xc00042f258</t>
   </si>
   <si>
     <t>10-22-04</t>
   </si>
   <si>
-    <t>0xc0005015a0</t>
-  </si>
-  <si>
-    <t>0xc000501590</t>
-  </si>
-  <si>
-    <t>0xc0005015b0</t>
-  </si>
-  <si>
-    <t>0xc0005015c0</t>
-  </si>
-  <si>
-    <t>0xc0005015d0</t>
-  </si>
-  <si>
-    <t>0xc000506f90</t>
-  </si>
-  <si>
-    <t>0xc000506fa0</t>
+    <t>0xc000200170</t>
+  </si>
+  <si>
+    <t>0xc000200160</t>
+  </si>
+  <si>
+    <t>0xc000200180</t>
+  </si>
+  <si>
+    <t>0xc000200190</t>
+  </si>
+  <si>
+    <t>0xc0002001a0</t>
+  </si>
+  <si>
+    <t>0xc00042f270</t>
+  </si>
+  <si>
+    <t>0xc00042f280</t>
   </si>
   <si>
     <t>10-22-05</t>
   </si>
   <si>
-    <t>0xc0005015f0</t>
-  </si>
-  <si>
-    <t>0xc0005015e0</t>
-  </si>
-  <si>
-    <t>0xc000501600</t>
-  </si>
-  <si>
-    <t>0xc000501610</t>
-  </si>
-  <si>
-    <t>0xc000501620</t>
-  </si>
-  <si>
-    <t>0xc000506fc0</t>
-  </si>
-  <si>
-    <t>0xc000506fd0</t>
+    <t>0xc0002001d0</t>
+  </si>
+  <si>
+    <t>0xc0002001c0</t>
+  </si>
+  <si>
+    <t>0xc0002001e0</t>
+  </si>
+  <si>
+    <t>0xc0002001f0</t>
+  </si>
+  <si>
+    <t>0xc000200200</t>
+  </si>
+  <si>
+    <t>0xc00042f2a0</t>
+  </si>
+  <si>
+    <t>0xc00042f2b0</t>
   </si>
   <si>
     <t>10-22-06</t>
   </si>
   <si>
-    <t>0xc000501640</t>
-  </si>
-  <si>
-    <t>0xc000501630</t>
-  </si>
-  <si>
-    <t>0xc000501650</t>
-  </si>
-  <si>
-    <t>0xc000501660</t>
-  </si>
-  <si>
-    <t>0xc000501670</t>
-  </si>
-  <si>
-    <t>0xc000506ff0</t>
-  </si>
-  <si>
-    <t>0xc000507000</t>
+    <t>0xc000200230</t>
+  </si>
+  <si>
+    <t>0xc000200220</t>
+  </si>
+  <si>
+    <t>0xc000200240</t>
+  </si>
+  <si>
+    <t>0xc000200250</t>
+  </si>
+  <si>
+    <t>0xc000200260</t>
+  </si>
+  <si>
+    <t>0xc00042f2d0</t>
+  </si>
+  <si>
+    <t>0xc00042f2e0</t>
   </si>
   <si>
     <t>10-22-07</t>
   </si>
   <si>
-    <t>0xc000501690</t>
-  </si>
-  <si>
-    <t>0xc000501680</t>
-  </si>
-  <si>
-    <t>0xc0005016a0</t>
-  </si>
-  <si>
-    <t>0xc0005016b0</t>
-  </si>
-  <si>
-    <t>0xc0005016c0</t>
-  </si>
-  <si>
-    <t>0xc000507020</t>
-  </si>
-  <si>
-    <t>0xc000507030</t>
+    <t>0xc000200290</t>
+  </si>
+  <si>
+    <t>0xc000200280</t>
+  </si>
+  <si>
+    <t>0xc0002002a0</t>
+  </si>
+  <si>
+    <t>0xc0002002b0</t>
+  </si>
+  <si>
+    <t>0xc0002002c0</t>
+  </si>
+  <si>
+    <t>0xc00042f300</t>
+  </si>
+  <si>
+    <t>0xc00042f310</t>
   </si>
   <si>
     <t>10-22-08</t>
   </si>
   <si>
-    <t>0xc0005016e0</t>
-  </si>
-  <si>
-    <t>0xc0005016d0</t>
-  </si>
-  <si>
-    <t>0xc0005016f0</t>
-  </si>
-  <si>
-    <t>0xc000501700</t>
-  </si>
-  <si>
-    <t>0xc000501710</t>
-  </si>
-  <si>
-    <t>0xc000507050</t>
-  </si>
-  <si>
-    <t>0xc000507060</t>
+    <t>0xc0002002f0</t>
+  </si>
+  <si>
+    <t>0xc0002002e0</t>
+  </si>
+  <si>
+    <t>0xc000200300</t>
+  </si>
+  <si>
+    <t>0xc000200310</t>
+  </si>
+  <si>
+    <t>0xc000200320</t>
+  </si>
+  <si>
+    <t>0xc00042f330</t>
+  </si>
+  <si>
+    <t>0xc00042f340</t>
   </si>
   <si>
     <t>10-22-09</t>
   </si>
   <si>
-    <t>0xc000501730</t>
-  </si>
-  <si>
-    <t>0xc000501720</t>
-  </si>
-  <si>
-    <t>0xc000501740</t>
-  </si>
-  <si>
-    <t>0xc000501750</t>
-  </si>
-  <si>
-    <t>0xc000501760</t>
-  </si>
-  <si>
-    <t>0xc000507080</t>
-  </si>
-  <si>
-    <t>0xc000507090</t>
+    <t>0xc000200350</t>
+  </si>
+  <si>
+    <t>0xc000200340</t>
+  </si>
+  <si>
+    <t>0xc000200360</t>
+  </si>
+  <si>
+    <t>0xc000200370</t>
+  </si>
+  <si>
+    <t>0xc000200380</t>
+  </si>
+  <si>
+    <t>0xc00042f360</t>
+  </si>
+  <si>
+    <t>0xc00042f370</t>
   </si>
   <si>
     <t>10-22-10</t>
   </si>
   <si>
-    <t>0xc000501780</t>
-  </si>
-  <si>
-    <t>0xc000501770</t>
-  </si>
-  <si>
-    <t>0xc000501790</t>
-  </si>
-  <si>
-    <t>0xc0005017a0</t>
-  </si>
-  <si>
-    <t>0xc0005017b0</t>
-  </si>
-  <si>
-    <t>0xc0005070a8</t>
-  </si>
-  <si>
-    <t>0xc0005070c8</t>
+    <t>0xc0002003b0</t>
+  </si>
+  <si>
+    <t>0xc0002003a0</t>
+  </si>
+  <si>
+    <t>0xc0002003c0</t>
+  </si>
+  <si>
+    <t>0xc0002003d0</t>
+  </si>
+  <si>
+    <t>0xc0002003e0</t>
+  </si>
+  <si>
+    <t>0xc00042f388</t>
+  </si>
+  <si>
+    <t>0xc00042f3a8</t>
   </si>
   <si>
     <t>10-22-11</t>
   </si>
   <si>
-    <t>0xc0005017d0</t>
-  </si>
-  <si>
-    <t>0xc0005017c0</t>
-  </si>
-  <si>
-    <t>0xc0005017e0</t>
-  </si>
-  <si>
-    <t>0xc0005017f0</t>
-  </si>
-  <si>
-    <t>0xc000501800</t>
-  </si>
-  <si>
-    <t>0xc0005070f0</t>
-  </si>
-  <si>
-    <t>0xc000507100</t>
+    <t>0xc000200410</t>
+  </si>
+  <si>
+    <t>0xc000200400</t>
+  </si>
+  <si>
+    <t>0xc000200420</t>
+  </si>
+  <si>
+    <t>0xc000200430</t>
+  </si>
+  <si>
+    <t>0xc000200440</t>
+  </si>
+  <si>
+    <t>0xc00042f3d0</t>
+  </si>
+  <si>
+    <t>0xc00042f3e0</t>
   </si>
   <si>
     <t>10-22-12</t>
   </si>
   <si>
-    <t>0xc000501820</t>
-  </si>
-  <si>
-    <t>0xc000501810</t>
-  </si>
-  <si>
-    <t>0xc000501830</t>
-  </si>
-  <si>
-    <t>0xc000501840</t>
-  </si>
-  <si>
-    <t>0xc000501850</t>
-  </si>
-  <si>
-    <t>0xc000507120</t>
-  </si>
-  <si>
-    <t>0xc000507150</t>
+    <t>0xc000200470</t>
+  </si>
+  <si>
+    <t>0xc000200460</t>
+  </si>
+  <si>
+    <t>0xc000200480</t>
+  </si>
+  <si>
+    <t>0xc000200490</t>
+  </si>
+  <si>
+    <t>0xc0002004a0</t>
+  </si>
+  <si>
+    <t>0xc00042f400</t>
+  </si>
+  <si>
+    <t>0xc00042f410</t>
   </si>
   <si>
     <t>10-22-13</t>
   </si>
   <si>
-    <t>0xc000501870</t>
-  </si>
-  <si>
-    <t>0xc000501860</t>
-  </si>
-  <si>
-    <t>0xc000501880</t>
-  </si>
-  <si>
-    <t>0xc000501890</t>
-  </si>
-  <si>
-    <t>0xc0005018a0</t>
-  </si>
-  <si>
-    <t>0xc000507188</t>
-  </si>
-  <si>
-    <t>0xc000507198</t>
+    <t>0xc0002004d0</t>
+  </si>
+  <si>
+    <t>0xc0002004c0</t>
+  </si>
+  <si>
+    <t>0xc0002004e0</t>
+  </si>
+  <si>
+    <t>0xc0002004f0</t>
+  </si>
+  <si>
+    <t>0xc000200500</t>
+  </si>
+  <si>
+    <t>0xc00042f428</t>
+  </si>
+  <si>
+    <t>0xc00042f438</t>
   </si>
   <si>
     <t>10-22-14</t>
   </si>
   <si>
-    <t>0xc0005018c0</t>
-  </si>
-  <si>
-    <t>0xc0005018b0</t>
-  </si>
-  <si>
-    <t>0xc0005018d0</t>
-  </si>
-  <si>
-    <t>0xc0005018e0</t>
-  </si>
-  <si>
-    <t>0xc0005018f0</t>
-  </si>
-  <si>
-    <t>0xc0005071c0</t>
-  </si>
-  <si>
-    <t>0xc0005071d0</t>
+    <t>0xc000200530</t>
+  </si>
+  <si>
+    <t>0xc000200520</t>
+  </si>
+  <si>
+    <t>0xc000200540</t>
+  </si>
+  <si>
+    <t>0xc000200550</t>
+  </si>
+  <si>
+    <t>0xc000200560</t>
+  </si>
+  <si>
+    <t>0xc00042f460</t>
+  </si>
+  <si>
+    <t>0xc00042f470</t>
   </si>
   <si>
     <t>10-22-15</t>
   </si>
   <si>
-    <t>0xc000501910</t>
-  </si>
-  <si>
-    <t>0xc000501900</t>
-  </si>
-  <si>
-    <t>0xc000501920</t>
-  </si>
-  <si>
-    <t>0xc000501930</t>
-  </si>
-  <si>
-    <t>0xc000501940</t>
-  </si>
-  <si>
-    <t>0xc0005071f0</t>
-  </si>
-  <si>
-    <t>0xc000507200</t>
+    <t>0xc000200590</t>
+  </si>
+  <si>
+    <t>0xc000200580</t>
+  </si>
+  <si>
+    <t>0xc0002005a0</t>
+  </si>
+  <si>
+    <t>0xc0002005b0</t>
+  </si>
+  <si>
+    <t>0xc0002005c0</t>
+  </si>
+  <si>
+    <t>0xc00042f490</t>
+  </si>
+  <si>
+    <t>0xc00042f4a0</t>
   </si>
   <si>
     <t>10-22-16</t>
   </si>
   <si>
-    <t>0xc000501960</t>
-  </si>
-  <si>
-    <t>0xc000501950</t>
-  </si>
-  <si>
-    <t>0xc000501970</t>
-  </si>
-  <si>
-    <t>0xc000501980</t>
-  </si>
-  <si>
-    <t>0xc000501990</t>
-  </si>
-  <si>
-    <t>0xc000507220</t>
-  </si>
-  <si>
-    <t>0xc000507230</t>
+    <t>0xc0002005f0</t>
+  </si>
+  <si>
+    <t>0xc0002005e0</t>
+  </si>
+  <si>
+    <t>0xc000200600</t>
+  </si>
+  <si>
+    <t>0xc000200610</t>
+  </si>
+  <si>
+    <t>0xc000200620</t>
+  </si>
+  <si>
+    <t>0xc00042f4c0</t>
+  </si>
+  <si>
+    <t>0xc00042f4d0</t>
   </si>
   <si>
     <t>10-22-17</t>
   </si>
   <si>
-    <t>0xc0005019b0</t>
-  </si>
-  <si>
-    <t>0xc0005019a0</t>
-  </si>
-  <si>
-    <t>0xc0005019c0</t>
-  </si>
-  <si>
-    <t>0xc0005019d0</t>
-  </si>
-  <si>
-    <t>0xc0005019e0</t>
-  </si>
-  <si>
-    <t>0xc000507250</t>
-  </si>
-  <si>
-    <t>0xc000507260</t>
+    <t>0xc000200650</t>
+  </si>
+  <si>
+    <t>0xc000200640</t>
+  </si>
+  <si>
+    <t>0xc000200660</t>
+  </si>
+  <si>
+    <t>0xc000200670</t>
+  </si>
+  <si>
+    <t>0xc000200680</t>
+  </si>
+  <si>
+    <t>0xc00042f4f0</t>
+  </si>
+  <si>
+    <t>0xc00042f500</t>
   </si>
   <si>
     <t>10-22-18</t>
   </si>
   <si>
-    <t>0xc000501a00</t>
-  </si>
-  <si>
-    <t>0xc0005019f0</t>
-  </si>
-  <si>
-    <t>0xc000501a10</t>
-  </si>
-  <si>
-    <t>0xc000501a20</t>
-  </si>
-  <si>
-    <t>0xc000501a30</t>
-  </si>
-  <si>
-    <t>0xc000507278</t>
-  </si>
-  <si>
-    <t>0xc000507288</t>
+    <t>0xc0002006b0</t>
+  </si>
+  <si>
+    <t>0xc0002006a0</t>
+  </si>
+  <si>
+    <t>0xc0002006c0</t>
+  </si>
+  <si>
+    <t>0xc0002006d0</t>
+  </si>
+  <si>
+    <t>0xc0002006e0</t>
+  </si>
+  <si>
+    <t>0xc00042f518</t>
+  </si>
+  <si>
+    <t>0xc00042f528</t>
   </si>
   <si>
     <t>123456</t>
@@ -1954,484 +1954,484 @@
     <t>&lt;nil&gt;</t>
   </si>
   <si>
-    <t>0xc000501a40</t>
-  </si>
-  <si>
-    <t>0xc000501a50</t>
-  </si>
-  <si>
-    <t>0xc000501a60</t>
-  </si>
-  <si>
-    <t>0xc000501a70</t>
-  </si>
-  <si>
-    <t>0xc000507298</t>
-  </si>
-  <si>
-    <t>0xc0005072a8</t>
+    <t>0xc000200700</t>
+  </si>
+  <si>
+    <t>0xc000200710</t>
+  </si>
+  <si>
+    <t>0xc000200720</t>
+  </si>
+  <si>
+    <t>0xc000200730</t>
+  </si>
+  <si>
+    <t>0xc00042f538</t>
+  </si>
+  <si>
+    <t>0xc00042f548</t>
   </si>
   <si>
     <t>CAP-112</t>
   </si>
   <si>
-    <t>0xc000501a90</t>
+    <t>0xc000200760</t>
   </si>
   <si>
     <t>H</t>
   </si>
   <si>
-    <t>0xc000501a80</t>
-  </si>
-  <si>
-    <t>0xc000501aa0</t>
-  </si>
-  <si>
-    <t>0xc000501ab0</t>
-  </si>
-  <si>
-    <t>0xc000501ac0</t>
-  </si>
-  <si>
-    <t>0xc0005072b8</t>
-  </si>
-  <si>
-    <t>0xc0005072c8</t>
+    <t>0xc000200750</t>
+  </si>
+  <si>
+    <t>0xc000200770</t>
+  </si>
+  <si>
+    <t>0xc000200780</t>
+  </si>
+  <si>
+    <t>0xc000200790</t>
+  </si>
+  <si>
+    <t>0xc00042f558</t>
+  </si>
+  <si>
+    <t>0xc00042f568</t>
   </si>
   <si>
     <t>CAP-144</t>
   </si>
   <si>
-    <t>0xc000501ae0</t>
+    <t>0xc0002007c0</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>0xc000501ad0</t>
-  </si>
-  <si>
-    <t>0xc000501af0</t>
-  </si>
-  <si>
-    <t>0xc000501b00</t>
-  </si>
-  <si>
-    <t>0xc000501b10</t>
-  </si>
-  <si>
-    <t>0xc0005072d8</t>
-  </si>
-  <si>
-    <t>0xc0005072f8</t>
+    <t>0xc0002007b0</t>
+  </si>
+  <si>
+    <t>0xc0002007d0</t>
+  </si>
+  <si>
+    <t>0xc0002007e0</t>
+  </si>
+  <si>
+    <t>0xc0002007f0</t>
+  </si>
+  <si>
+    <t>0xc00042f578</t>
+  </si>
+  <si>
+    <t>0xc00042f598</t>
   </si>
   <si>
     <t>CAP-198</t>
   </si>
   <si>
-    <t>0xc000501b30</t>
-  </si>
-  <si>
-    <t>0xc000501b20</t>
-  </si>
-  <si>
-    <t>0xc000501b40</t>
-  </si>
-  <si>
-    <t>0xc000501b50</t>
-  </si>
-  <si>
-    <t>0xc000501b60</t>
-  </si>
-  <si>
-    <t>0xc000507308</t>
-  </si>
-  <si>
-    <t>0xc000507328</t>
+    <t>0xc000200820</t>
+  </si>
+  <si>
+    <t>0xc000200810</t>
+  </si>
+  <si>
+    <t>0xc000200830</t>
+  </si>
+  <si>
+    <t>0xc000200840</t>
+  </si>
+  <si>
+    <t>0xc000200850</t>
+  </si>
+  <si>
+    <t>0xc00042f5a8</t>
+  </si>
+  <si>
+    <t>0xc00042f5c8</t>
   </si>
   <si>
     <t>CAP-205</t>
   </si>
   <si>
-    <t>0xc000501b80</t>
-  </si>
-  <si>
-    <t>0xc000501b70</t>
-  </si>
-  <si>
-    <t>0xc000501b90</t>
-  </si>
-  <si>
-    <t>0xc000501ba0</t>
-  </si>
-  <si>
-    <t>0xc000501bb0</t>
-  </si>
-  <si>
-    <t>0xc000507338</t>
-  </si>
-  <si>
-    <t>0xc000507358</t>
+    <t>0xc000200880</t>
+  </si>
+  <si>
+    <t>0xc000200870</t>
+  </si>
+  <si>
+    <t>0xc000200890</t>
+  </si>
+  <si>
+    <t>0xc0002008a0</t>
+  </si>
+  <si>
+    <t>0xc0002008b0</t>
+  </si>
+  <si>
+    <t>0xc00042f5d8</t>
+  </si>
+  <si>
+    <t>0xc00042f5f8</t>
   </si>
   <si>
     <t>CAP-225</t>
   </si>
   <si>
-    <t>0xc000501bd0</t>
-  </si>
-  <si>
-    <t>0xc000501bc0</t>
-  </si>
-  <si>
-    <t>0xc000501be0</t>
-  </si>
-  <si>
-    <t>0xc000501bf0</t>
-  </si>
-  <si>
-    <t>0xc000501c00</t>
-  </si>
-  <si>
-    <t>0xc000507368</t>
-  </si>
-  <si>
-    <t>0xc000507378</t>
+    <t>0xc0002008e0</t>
+  </si>
+  <si>
+    <t>0xc0002008d0</t>
+  </si>
+  <si>
+    <t>0xc0002008f0</t>
+  </si>
+  <si>
+    <t>0xc000200900</t>
+  </si>
+  <si>
+    <t>0xc000200910</t>
+  </si>
+  <si>
+    <t>0xc00042f608</t>
+  </si>
+  <si>
+    <t>0xc00042f618</t>
   </si>
   <si>
     <t>CAP-230</t>
   </si>
   <si>
-    <t>0xc000501c20</t>
-  </si>
-  <si>
-    <t>0xc000501c10</t>
-  </si>
-  <si>
-    <t>0xc000501c30</t>
-  </si>
-  <si>
-    <t>0xc000501c40</t>
-  </si>
-  <si>
-    <t>0xc000501c50</t>
-  </si>
-  <si>
-    <t>0xc000507388</t>
-  </si>
-  <si>
-    <t>0xc0005073a8</t>
+    <t>0xc000200940</t>
+  </si>
+  <si>
+    <t>0xc000200930</t>
+  </si>
+  <si>
+    <t>0xc000200950</t>
+  </si>
+  <si>
+    <t>0xc000200960</t>
+  </si>
+  <si>
+    <t>0xc000200970</t>
+  </si>
+  <si>
+    <t>0xc00042f628</t>
+  </si>
+  <si>
+    <t>0xc00042f648</t>
   </si>
   <si>
     <t>CAP-251</t>
   </si>
   <si>
-    <t>0xc000501c70</t>
-  </si>
-  <si>
-    <t>0xc000501c60</t>
-  </si>
-  <si>
-    <t>0xc000501c80</t>
-  </si>
-  <si>
-    <t>0xc000501c90</t>
-  </si>
-  <si>
-    <t>0xc000501ca0</t>
-  </si>
-  <si>
-    <t>0xc0005073b8</t>
-  </si>
-  <si>
-    <t>0xc0005073d8</t>
+    <t>0xc0002009a0</t>
+  </si>
+  <si>
+    <t>0xc000200990</t>
+  </si>
+  <si>
+    <t>0xc0002009b0</t>
+  </si>
+  <si>
+    <t>0xc0002009c0</t>
+  </si>
+  <si>
+    <t>0xc0002009d0</t>
+  </si>
+  <si>
+    <t>0xc00042f658</t>
+  </si>
+  <si>
+    <t>0xc00042f678</t>
   </si>
   <si>
     <t>CAP-260</t>
   </si>
   <si>
-    <t>0xc000501cc0</t>
-  </si>
-  <si>
-    <t>0xc000501cb0</t>
-  </si>
-  <si>
-    <t>0xc000501cd0</t>
-  </si>
-  <si>
-    <t>0xc000501ce0</t>
-  </si>
-  <si>
-    <t>0xc000501cf0</t>
-  </si>
-  <si>
-    <t>0xc0005073e8</t>
-  </si>
-  <si>
-    <t>0xc000507408</t>
+    <t>0xc000200a00</t>
+  </si>
+  <si>
+    <t>0xc0002009f0</t>
+  </si>
+  <si>
+    <t>0xc000200a10</t>
+  </si>
+  <si>
+    <t>0xc000200a20</t>
+  </si>
+  <si>
+    <t>0xc000200a30</t>
+  </si>
+  <si>
+    <t>0xc00042f688</t>
+  </si>
+  <si>
+    <t>0xc00042f6a8</t>
   </si>
   <si>
     <t>CAP-263</t>
   </si>
   <si>
-    <t>0xc000501d10</t>
-  </si>
-  <si>
-    <t>0xc000501d00</t>
-  </si>
-  <si>
-    <t>0xc000501d20</t>
-  </si>
-  <si>
-    <t>0xc000501d30</t>
-  </si>
-  <si>
-    <t>0xc000501d40</t>
-  </si>
-  <si>
-    <t>0xc000507430</t>
-  </si>
-  <si>
-    <t>0xc000507440</t>
+    <t>0xc000200a60</t>
+  </si>
+  <si>
+    <t>0xc000200a50</t>
+  </si>
+  <si>
+    <t>0xc000200a70</t>
+  </si>
+  <si>
+    <t>0xc000200a80</t>
+  </si>
+  <si>
+    <t>0xc000200a90</t>
+  </si>
+  <si>
+    <t>0xc00042f6d0</t>
+  </si>
+  <si>
+    <t>0xc00042f6e0</t>
   </si>
   <si>
     <t>CAP-272</t>
   </si>
   <si>
-    <t>0xc000501d60</t>
-  </si>
-  <si>
-    <t>0xc000501d50</t>
-  </si>
-  <si>
-    <t>0xc000501d70</t>
-  </si>
-  <si>
-    <t>0xc000501d80</t>
-  </si>
-  <si>
-    <t>0xc000501d90</t>
-  </si>
-  <si>
-    <t>0xc000507460</t>
-  </si>
-  <si>
-    <t>0xc000507470</t>
+    <t>0xc000200ac0</t>
+  </si>
+  <si>
+    <t>0xc000200ab0</t>
+  </si>
+  <si>
+    <t>0xc000200ad0</t>
+  </si>
+  <si>
+    <t>0xc000200ae0</t>
+  </si>
+  <si>
+    <t>0xc000200af0</t>
+  </si>
+  <si>
+    <t>0xc00042f700</t>
+  </si>
+  <si>
+    <t>0xc00042f710</t>
   </si>
   <si>
     <t>CAP-312</t>
   </si>
   <si>
-    <t>0xc000501db0</t>
-  </si>
-  <si>
-    <t>0xc000501da0</t>
-  </si>
-  <si>
-    <t>0xc000501dc0</t>
-  </si>
-  <si>
-    <t>0xc000501dd0</t>
-  </si>
-  <si>
-    <t>0xc000501de0</t>
-  </si>
-  <si>
-    <t>0xc000507498</t>
-  </si>
-  <si>
-    <t>0xc0005074b0</t>
+    <t>0xc000200b20</t>
+  </si>
+  <si>
+    <t>0xc000200b10</t>
+  </si>
+  <si>
+    <t>0xc000200b30</t>
+  </si>
+  <si>
+    <t>0xc000200b40</t>
+  </si>
+  <si>
+    <t>0xc000200b50</t>
+  </si>
+  <si>
+    <t>0xc00042f738</t>
+  </si>
+  <si>
+    <t>0xc00042f750</t>
   </si>
   <si>
     <t>CAP-313</t>
   </si>
   <si>
-    <t>0xc000501e00</t>
-  </si>
-  <si>
-    <t>0xc000501df0</t>
-  </si>
-  <si>
-    <t>0xc000501e10</t>
-  </si>
-  <si>
-    <t>0xc000501e20</t>
-  </si>
-  <si>
-    <t>0xc000501e30</t>
-  </si>
-  <si>
-    <t>0xc0005074c8</t>
-  </si>
-  <si>
-    <t>0xc0005074e0</t>
+    <t>0xc000200b80</t>
+  </si>
+  <si>
+    <t>0xc000200b70</t>
+  </si>
+  <si>
+    <t>0xc000200b90</t>
+  </si>
+  <si>
+    <t>0xc000200ba0</t>
+  </si>
+  <si>
+    <t>0xc000200bb0</t>
+  </si>
+  <si>
+    <t>0xc00042f768</t>
+  </si>
+  <si>
+    <t>0xc00042f780</t>
   </si>
   <si>
     <t>CAP-314</t>
   </si>
   <si>
-    <t>0xc000501e50</t>
-  </si>
-  <si>
-    <t>0xc000501e40</t>
-  </si>
-  <si>
-    <t>0xc000501e60</t>
-  </si>
-  <si>
-    <t>0xc000501e70</t>
-  </si>
-  <si>
-    <t>0xc000501e80</t>
-  </si>
-  <si>
-    <t>0xc0005074f8</t>
-  </si>
-  <si>
-    <t>0xc000507510</t>
+    <t>0xc000200be0</t>
+  </si>
+  <si>
+    <t>0xc000200bd0</t>
+  </si>
+  <si>
+    <t>0xc000200bf0</t>
+  </si>
+  <si>
+    <t>0xc000200c00</t>
+  </si>
+  <si>
+    <t>0xc000200c10</t>
+  </si>
+  <si>
+    <t>0xc00042f798</t>
+  </si>
+  <si>
+    <t>0xc00042f7b0</t>
   </si>
   <si>
     <t>CAP-316</t>
   </si>
   <si>
-    <t>0xc000501ea0</t>
-  </si>
-  <si>
-    <t>0xc000501e90</t>
-  </si>
-  <si>
-    <t>0xc000501eb0</t>
-  </si>
-  <si>
-    <t>0xc000501ec0</t>
-  </si>
-  <si>
-    <t>0xc000501ed0</t>
-  </si>
-  <si>
-    <t>0xc000507528</t>
-  </si>
-  <si>
-    <t>0xc000507540</t>
+    <t>0xc000200c40</t>
+  </si>
+  <si>
+    <t>0xc000200c30</t>
+  </si>
+  <si>
+    <t>0xc000200c50</t>
+  </si>
+  <si>
+    <t>0xc000200c60</t>
+  </si>
+  <si>
+    <t>0xc000200c70</t>
+  </si>
+  <si>
+    <t>0xc00042f7c8</t>
+  </si>
+  <si>
+    <t>0xc00042f7e0</t>
   </si>
   <si>
     <t>CAP-317</t>
   </si>
   <si>
-    <t>0xc000501ef0</t>
-  </si>
-  <si>
-    <t>0xc000501ee0</t>
-  </si>
-  <si>
-    <t>0xc000501f00</t>
-  </si>
-  <si>
-    <t>0xc000501f10</t>
-  </si>
-  <si>
-    <t>0xc000501f20</t>
-  </si>
-  <si>
-    <t>0xc000507558</t>
-  </si>
-  <si>
-    <t>0xc000507570</t>
+    <t>0xc000200ca0</t>
+  </si>
+  <si>
+    <t>0xc000200c90</t>
+  </si>
+  <si>
+    <t>0xc000200cb0</t>
+  </si>
+  <si>
+    <t>0xc000200cc0</t>
+  </si>
+  <si>
+    <t>0xc000200cd0</t>
+  </si>
+  <si>
+    <t>0xc00042f7f8</t>
+  </si>
+  <si>
+    <t>0xc00042f810</t>
   </si>
   <si>
     <t>CAP-320</t>
   </si>
   <si>
-    <t>0xc000501f40</t>
-  </si>
-  <si>
-    <t>0xc000501f30</t>
-  </si>
-  <si>
-    <t>0xc000501f50</t>
-  </si>
-  <si>
-    <t>0xc000501f60</t>
-  </si>
-  <si>
-    <t>0xc000501f70</t>
-  </si>
-  <si>
-    <t>0xc000507590</t>
-  </si>
-  <si>
-    <t>0xc0005075a0</t>
+    <t>0xc000200d00</t>
+  </si>
+  <si>
+    <t>0xc000200cf0</t>
+  </si>
+  <si>
+    <t>0xc000200d10</t>
+  </si>
+  <si>
+    <t>0xc000200d20</t>
+  </si>
+  <si>
+    <t>0xc000200d30</t>
+  </si>
+  <si>
+    <t>0xc00042f830</t>
+  </si>
+  <si>
+    <t>0xc00042f840</t>
   </si>
   <si>
     <t>CAP-321</t>
   </si>
   <si>
-    <t>0xc000501f90</t>
-  </si>
-  <si>
-    <t>0xc000501f80</t>
-  </si>
-  <si>
-    <t>0xc000501fa0</t>
-  </si>
-  <si>
-    <t>0xc000501fb0</t>
-  </si>
-  <si>
-    <t>0xc000501fc0</t>
-  </si>
-  <si>
-    <t>0xc0005075c0</t>
-  </si>
-  <si>
-    <t>0xc0005075d0</t>
+    <t>0xc000200d60</t>
+  </si>
+  <si>
+    <t>0xc000200d50</t>
+  </si>
+  <si>
+    <t>0xc000200d70</t>
+  </si>
+  <si>
+    <t>0xc000200d80</t>
+  </si>
+  <si>
+    <t>0xc000200d90</t>
+  </si>
+  <si>
+    <t>0xc00042f860</t>
+  </si>
+  <si>
+    <t>0xc00042f870</t>
   </si>
   <si>
     <t>CAP-322</t>
   </si>
   <si>
-    <t>0xc000501fe0</t>
-  </si>
-  <si>
-    <t>0xc000501fd0</t>
-  </si>
-  <si>
-    <t>0xc000501ff0</t>
-  </si>
-  <si>
-    <t>0xc00009c000</t>
-  </si>
-  <si>
-    <t>0xc00009c010</t>
-  </si>
-  <si>
-    <t>0xc0005075f8</t>
-  </si>
-  <si>
-    <t>0xc000507608</t>
+    <t>0xc000200dc0</t>
+  </si>
+  <si>
+    <t>0xc000200db0</t>
+  </si>
+  <si>
+    <t>0xc000200dd0</t>
+  </si>
+  <si>
+    <t>0xc000200de0</t>
+  </si>
+  <si>
+    <t>0xc000200df0</t>
+  </si>
+  <si>
+    <t>0xc00042f898</t>
+  </si>
+  <si>
+    <t>0xc00042f8a8</t>
   </si>
   <si>
     <t>CAP-323</t>
   </si>
   <si>
-    <t>0xc00009c030</t>
-  </si>
-  <si>
-    <t>0xc00009c020</t>
-  </si>
-  <si>
-    <t>0xc00009c040</t>
-  </si>
-  <si>
-    <t>0xc00009c050</t>
-  </si>
-  <si>
-    <t>0xc00009c060</t>
-  </si>
-  <si>
-    <t>0xc000507630</t>
-  </si>
-  <si>
-    <t>0xc000507648</t>
+    <t>0xc000200e20</t>
+  </si>
+  <si>
+    <t>0xc000200e10</t>
+  </si>
+  <si>
+    <t>0xc000200e30</t>
+  </si>
+  <si>
+    <t>0xc000200e40</t>
+  </si>
+  <si>
+    <t>0xc000200e50</t>
+  </si>
+  <si>
+    <t>0xc00042f8d0</t>
+  </si>
+  <si>
+    <t>0xc00042f8e8</t>
   </si>
 </sst>
 </file>

</xml_diff>